<commit_message>
Updating step10 to .ris
</commit_message>
<xml_diff>
--- a/scripts/data/calibration_r1_205.xlsx
+++ b/scripts/data/calibration_r1_205.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I206"/>
+  <dimension ref="A1:E206"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,19 +416,7 @@
         <v>Title</v>
       </c>
       <c r="E1" t="str">
-        <v>Journal</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Info</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Authors</v>
-      </c>
-      <c r="H1" t="str">
         <v>Year</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Ref. Type</v>
       </c>
     </row>
     <row r="2">
@@ -445,19 +433,7 @@
         <v>Combined effect of fertilizer micro-dosing and intercropped millet/cowpea effect on agronomic and economic advantages in prone Sahel area, Niger</v>
       </c>
       <c r="E2" t="str">
-        <v>Discover Sustainability</v>
-      </c>
-      <c r="F2" t="str">
-        <v/>
-      </c>
-      <c r="G2" t="str">
-        <v xml:space="preserve">Abdoul-Karim Toudou Daouda; Sanoussi Atta; Soulé Moussa; Yacoubou Bakasso; </v>
-      </c>
-      <c r="H2" t="str">
         <v>2022</v>
-      </c>
-      <c r="I2" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="3">
@@ -474,19 +450,7 @@
         <v>Pastoralists' perceptions of feed scarcity and livestock poisoning in southern rangelands, Ethiopia</v>
       </c>
       <c r="E3" t="str">
-        <v>Tropical Animal Health and Production</v>
-      </c>
-      <c r="F3" t="str">
-        <v/>
-      </c>
-      <c r="G3" t="str">
-        <v xml:space="preserve">Abebe Aster; Eik Lars Olav; Holand Øystein; Ådnøy Tormod; Tolera Adugna; </v>
-      </c>
-      <c r="H3" t="str">
         <v>2012</v>
-      </c>
-      <c r="I3" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="4">
@@ -503,19 +467,7 @@
         <v>Adapting the current mass mobilization approach in Ethiopia to enhance its impact on sustainable land management: Lessons from the Sago-kara watershed</v>
       </c>
       <c r="E4" t="str">
-        <v>Journal of Environmental Management</v>
-      </c>
-      <c r="F4" t="str">
-        <v/>
-      </c>
-      <c r="G4" t="str">
-        <v xml:space="preserve">Abi Meskerem; Kessler Aad; Oosterveer Peter; Tolossa Degefa; </v>
-      </c>
-      <c r="H4" t="str">
         <v>2019</v>
-      </c>
-      <c r="I4" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="5">
@@ -532,19 +484,7 @@
         <v>The Impacts of Climate Change on the Livelihood of Arable Crop Farmers in Southwest, Nigeria</v>
       </c>
       <c r="E5" t="str">
-        <v>Climate Change Management</v>
-      </c>
-      <c r="F5" t="str">
-        <v/>
-      </c>
-      <c r="G5" t="str">
-        <v xml:space="preserve">Abiona B G; Fakoya E O; Esun J; </v>
-      </c>
-      <c r="H5" t="str">
         <v>2016</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="6">
@@ -561,19 +501,7 @@
         <v>Agricultural water demand, water quality and crop suitability in Souk-Alkhamis Al-Khums, Libya</v>
       </c>
       <c r="E6" t="str">
-        <v>Iop Conference Series Earth and Environmental Science</v>
-      </c>
-      <c r="F6" t="str">
-        <v/>
-      </c>
-      <c r="G6" t="str">
-        <v xml:space="preserve">Abunnour Mohamed Ali; Hashim Noorazuan Bin Md; Bin Jaafar; Mokhtar; </v>
-      </c>
-      <c r="H6" t="str">
         <v>2016</v>
-      </c>
-      <c r="I6" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="7">
@@ -590,19 +518,7 @@
         <v>Current knowledge on Amaranthus spp.: Research avenues for improved nutritional value and yield in leafy amaranths in sub-Saharan Africa</v>
       </c>
       <c r="E7" t="str">
-        <v>Euphytica</v>
-      </c>
-      <c r="F7" t="str">
-        <v/>
-      </c>
-      <c r="G7" t="str">
-        <v xml:space="preserve">Achigan-Dako Enoch G; Sogbohossou Olga E. D; Maundu Patrick; </v>
-      </c>
-      <c r="H7" t="str">
         <v>2014</v>
-      </c>
-      <c r="I7" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="8">
@@ -619,19 +535,7 @@
         <v>Effects of quality coffee production on smallholders’ adaptation to climate change in Yirgacheffe, Southern Ethiopia</v>
       </c>
       <c r="E8" t="str">
-        <v>International Journal of Climate Change Strategies and Management</v>
-      </c>
-      <c r="F8" t="str">
-        <v/>
-      </c>
-      <c r="G8" t="str">
-        <v xml:space="preserve">Adane Asnake; Bewket Woldeamlak; </v>
-      </c>
-      <c r="H8" t="str">
         <v>2021</v>
-      </c>
-      <c r="I8" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="9">
@@ -648,19 +552,7 @@
         <v>Adaptation strategies of citrus and tomato farmers towards the effect of climate change in Nigeria</v>
       </c>
       <c r="E9" t="str">
-        <v>Vulnerability of Agriculture Water and Fisheries to Climate Change Toward Sustainable Adaptation Strategies</v>
-      </c>
-      <c r="F9" t="str">
-        <v/>
-      </c>
-      <c r="G9" t="str">
-        <v xml:space="preserve">Adebisi-Adelani O; Oyesola O B; </v>
-      </c>
-      <c r="H9" t="str">
         <v>2014</v>
-      </c>
-      <c r="I9" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="10">
@@ -677,19 +569,7 @@
         <v>Global assessment of technological innovation for climate change adaptation and mitigation in developing world</v>
       </c>
       <c r="E10" t="str">
-        <v>Journal of Environmental Management</v>
-      </c>
-      <c r="F10" t="str">
-        <v/>
-      </c>
-      <c r="G10" t="str">
-        <v xml:space="preserve">Adenle Ademola A; Azadi Hossein; Arbiol Joseph; </v>
-      </c>
-      <c r="H10" t="str">
         <v>2015</v>
-      </c>
-      <c r="I10" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="11">
@@ -706,19 +586,7 @@
         <v>Simultaneous adoption of catastrophic risk management tools in aquaculture: A study of floodplain areas of Bangladesh</v>
       </c>
       <c r="E11" t="str">
-        <v>International Journal of Disaster Risk Reduction</v>
-      </c>
-      <c r="F11" t="str">
-        <v/>
-      </c>
-      <c r="G11" t="str">
-        <v xml:space="preserve">Adnan K M Mehedi; Xicang Zhao; Sarker Swati Anindita; Jiying Wu; Alamgir Md Shah; </v>
-      </c>
-      <c r="H11" t="str">
         <v>2025</v>
-      </c>
-      <c r="I11" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="12">
@@ -735,19 +603,7 @@
         <v>Agroecology and the Human Rights-Based Approach: Transforming Food and Agricultural Systems to Improve Small Farmers’ Livelihoods</v>
       </c>
       <c r="E12" t="str">
-        <v>Food Security Issues and Challenges</v>
-      </c>
-      <c r="F12" t="str">
-        <v/>
-      </c>
-      <c r="G12" t="str">
-        <v/>
-      </c>
-      <c r="H12" t="str">
         <v>2021</v>
-      </c>
-      <c r="I12" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="13">
@@ -764,19 +620,7 @@
         <v>Conducting a Tailored and Localised Marine Heat Wave Risk Assessment for Vanuatu Fisheries</v>
       </c>
       <c r="E13" t="str">
-        <v>Climate</v>
-      </c>
-      <c r="F13" t="str">
-        <v/>
-      </c>
-      <c r="G13" t="str">
-        <v xml:space="preserve">Aitkenhead Isabella; Kuleshov Yuriy; Sun Chayn; Choy Suelynn; </v>
-      </c>
-      <c r="H13" t="str">
         <v>2024</v>
-      </c>
-      <c r="I13" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="14">
@@ -793,19 +637,7 @@
         <v>The effects of addressing gender norms and access to resources on gender equality in climate-affected agrifood systems in Bangladesh</v>
       </c>
       <c r="E14" t="str">
-        <v>International Journal of Agricultural Sustainability</v>
-      </c>
-      <c r="F14" t="str">
-        <v/>
-      </c>
-      <c r="G14" t="str">
-        <v xml:space="preserve">Akhter Sadika; Lecoutere Els; Kihoro Esther; Kamruzzaman Mohammed; Dey Durjoy; </v>
-      </c>
-      <c r="H14" t="str">
         <v>2025</v>
-      </c>
-      <c r="I14" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="15">
@@ -822,19 +654,7 @@
         <v>Impact of climate smart agriculture on households’ resilience and vulnerability: An example from Central Rift Valley, Ethiopia</v>
       </c>
       <c r="E15" t="str">
-        <v>Climate Resilience and Sustainability</v>
-      </c>
-      <c r="F15" t="str">
-        <v/>
-      </c>
-      <c r="G15" t="str">
-        <v xml:space="preserve">Ali Hussien; Menza Mesfin; Hagos Fitsum; Haileslassie Amare; </v>
-      </c>
-      <c r="H15" t="str">
         <v>2023</v>
-      </c>
-      <c r="I15" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="16">
@@ -851,19 +671,7 @@
         <v>Unveiling the determinants of climate change adaptation among small Landholders: Insights from a Mountainous Region in Pakistan</v>
       </c>
       <c r="E16" t="str">
-        <v>Climate Services</v>
-      </c>
-      <c r="F16" t="str">
-        <v/>
-      </c>
-      <c r="G16" t="str">
-        <v xml:space="preserve">Ali Iftikhar; Shah Ashfaq Ahmad; Alotaibi Bader Alhafi; Xu Chong; Ali Amjad; Ali Yousuf; </v>
-      </c>
-      <c r="H16" t="str">
         <v>2025</v>
-      </c>
-      <c r="I16" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="17">
@@ -880,19 +688,7 @@
         <v>Drought perception and field-level adaptation strategies of farming households in drought-prone areas of Afghanistan</v>
       </c>
       <c r="E17" t="str">
-        <v>International Journal of Disaster Risk Reduction</v>
-      </c>
-      <c r="F17" t="str">
-        <v/>
-      </c>
-      <c r="G17" t="str">
-        <v xml:space="preserve">Aliyar Qurban; Zulfiqar Farhad; Datta Avishek; Kuwornu John K.M; Shrestha Sangam; </v>
-      </c>
-      <c r="H17" t="str">
         <v>2022</v>
-      </c>
-      <c r="I17" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="18">
@@ -909,19 +705,7 @@
         <v>Farmers’ beliefs and concerns about climate change: An assessment from southern Saudi Arabia</v>
       </c>
       <c r="E18" t="str">
-        <v>Agriculture Switzerland</v>
-      </c>
-      <c r="F18" t="str">
-        <v/>
-      </c>
-      <c r="G18" t="str">
-        <v xml:space="preserve">Alotaibi Bader Alhafi; Kassem Hazem S; Nayak Roshan K; Muddassir Muhammad; </v>
-      </c>
-      <c r="H18" t="str">
         <v>2020</v>
-      </c>
-      <c r="I18" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="19">
@@ -938,19 +722,7 @@
         <v>Dynamics and Determinants of Farmers’ Perceptions about Causes and Impacts of Climate Change on Agriculture in Saudi Arabia: Implications for Adaptation, Mitigation, and Sustainability</v>
       </c>
       <c r="E19" t="str">
-        <v>Atmosphere</v>
-      </c>
-      <c r="F19" t="str">
-        <v/>
-      </c>
-      <c r="G19" t="str">
-        <v xml:space="preserve">Alotaibi Bader Alhafi; Abbas Azhar; Ullah Raza; Azeem Muhammad Imran; Samie Abdus; Muddassir Muhammad; Dabiah Abduaziz Thabet; Raid Moodhi; Sadaf Tahira; </v>
-      </c>
-      <c r="H19" t="str">
         <v>2023</v>
-      </c>
-      <c r="I19" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="20">
@@ -967,19 +739,7 @@
         <v>Yield stability and phenotypic plasticity of Populus spp. clones growing in environmental gradients: I-yield stability under field conditions</v>
       </c>
       <c r="E20" t="str">
-        <v>Forest Ecology and Management</v>
-      </c>
-      <c r="F20" t="str">
-        <v/>
-      </c>
-      <c r="G20" t="str">
-        <v xml:space="preserve">Alvarez Javier A; Cortizo Silvia C; Gyenge Javier E; </v>
-      </c>
-      <c r="H20" t="str">
         <v>2020</v>
-      </c>
-      <c r="I20" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="21">
@@ -996,19 +756,7 @@
         <v>Building climate resilience in the MENA region: a feminist political ecology of agroecology and neglected and underutilized crop species</v>
       </c>
       <c r="E21" t="str">
-        <v>Agriculture and Human Values</v>
-      </c>
-      <c r="F21" t="str">
-        <v/>
-      </c>
-      <c r="G21" t="str">
-        <v xml:space="preserve">Amoak Daniel; Najjar Dina; Nyantakyi-Frimpong Hanson; Amil Rola El; Maalouf Fouad; Abderrazek Jilal; </v>
-      </c>
-      <c r="H21" t="str">
         <v>2026</v>
-      </c>
-      <c r="I21" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="22">
@@ -1025,19 +773,7 @@
         <v>Vehicular livestock mobility in West Africa: Seasonal traffic flows of cattle, sheep, and goats across bamako</v>
       </c>
       <c r="E22" t="str">
-        <v>Sustainability Switzerland</v>
-      </c>
-      <c r="F22" t="str">
-        <v/>
-      </c>
-      <c r="G22" t="str">
-        <v xml:space="preserve">Amprako Louis; Karg Hanna; Roessler Regina; Provost Jennifer; Akoto-Danso Edmund Kyei; Sidibe Seydou; Buerkert Andreas; </v>
-      </c>
-      <c r="H22" t="str">
         <v>2021</v>
-      </c>
-      <c r="I22" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="23">
@@ -1054,19 +790,7 @@
         <v>Local Adaptation Strategies in Combating Flooding in Fisheries and Aquaculture in Nigeria</v>
       </c>
       <c r="E23" t="str">
-        <v>Handbook of Climate Change Management Research Leadership Transformation</v>
-      </c>
-      <c r="F23" t="str">
-        <v/>
-      </c>
-      <c r="G23" t="str">
-        <v xml:space="preserve">Areola Foluke; </v>
-      </c>
-      <c r="H23" t="str">
         <v>2021</v>
-      </c>
-      <c r="I23" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="24">
@@ -1083,19 +807,7 @@
         <v>Livelihood vulnerability assessment to climate change and variability: the case of farm households in South-East Tunisia</v>
       </c>
       <c r="E24" t="str">
-        <v>Environment Development and Sustainability</v>
-      </c>
-      <c r="F24" t="str">
-        <v/>
-      </c>
-      <c r="G24" t="str">
-        <v xml:space="preserve">Aribi Fatma; Sghaier Mongi; </v>
-      </c>
-      <c r="H24" t="str">
         <v>2021</v>
-      </c>
-      <c r="I24" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="25">
@@ -1112,19 +824,7 @@
         <v>Assessing the impacts of climate change on land productivity in indian crop agriculture: An evidence from panel data analysis</v>
       </c>
       <c r="E25" t="str">
-        <v>Journal of Agricultural Science and Technology</v>
-      </c>
-      <c r="F25" t="str">
-        <v/>
-      </c>
-      <c r="G25" t="str">
-        <v/>
-      </c>
-      <c r="H25" t="str">
         <v>2016</v>
-      </c>
-      <c r="I25" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="26">
@@ -1141,19 +841,7 @@
         <v>Climate change resiliency choices of small-scale farmers in Cameroon: determinants and policy implications</v>
       </c>
       <c r="E26" t="str">
-        <v>Journal of Environmental Management</v>
-      </c>
-      <c r="F26" t="str">
-        <v/>
-      </c>
-      <c r="G26" t="str">
-        <v xml:space="preserve">Awazi Nyong Princely; Tchamba Martin Ngankam; Avana Tientcheu Marie-Louise; </v>
-      </c>
-      <c r="H26" t="str">
         <v>2019</v>
-      </c>
-      <c r="I26" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="27">
@@ -1170,19 +858,7 @@
         <v>Map analysis of soil erodibility rates and gully erosion sites in Anambra State, South Eastern Nigeria</v>
       </c>
       <c r="E27" t="str">
-        <v>Open Geosciences</v>
-      </c>
-      <c r="F27" t="str">
-        <v/>
-      </c>
-      <c r="G27" t="str">
-        <v xml:space="preserve">Ayadiuno Romanus Udegbunam; Ndulue Dominic Chukwuka; Ezeh Christopher Uche; </v>
-      </c>
-      <c r="H27" t="str">
         <v>2025</v>
-      </c>
-      <c r="I27" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="28">
@@ -1199,19 +875,7 @@
         <v>Effect of climate warming on maize production in Timor-Leste: Interaction with nitrogen supply</v>
       </c>
       <c r="E28" t="str">
-        <v>Crop and Pasture Science</v>
-      </c>
-      <c r="F28" t="str">
-        <v/>
-      </c>
-      <c r="G28" t="str">
-        <v xml:space="preserve">Bacon Samuel A; Mau Raimundo; Neto Florindo M; Williams Robert L; Turner Neil C; </v>
-      </c>
-      <c r="H28" t="str">
         <v>2016</v>
-      </c>
-      <c r="I28" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="29">
@@ -1228,19 +892,7 @@
         <v>What drives farmers to adopt farm-level adaptation practices to climate extremes: Empirical evidence from Odisha, India</v>
       </c>
       <c r="E29" t="str">
-        <v>International Journal of Disaster Risk Reduction</v>
-      </c>
-      <c r="F29" t="str">
-        <v/>
-      </c>
-      <c r="G29" t="str">
-        <v xml:space="preserve">Bahinipati Chandra Sekhar; Venkatachalam L; </v>
-      </c>
-      <c r="H29" t="str">
         <v>2015</v>
-      </c>
-      <c r="I29" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="30">
@@ -1257,19 +909,7 @@
         <v>Assessing heat exposure and its effects on farmer health, harvest yields, and nutrition: a study protocol for Burkina Faso and Kenya</v>
       </c>
       <c r="E30" t="str">
-        <v>Global Health Action</v>
-      </c>
-      <c r="F30" t="str">
-        <v/>
-      </c>
-      <c r="G30" t="str">
-        <v xml:space="preserve">Barteit Sandra; Ouédraogo Windpanga Aristide; Müller Charlotte; Zabré Pascal; Traoré Issouf; Boudo Valentin; Sié Ali; Compaoré Guillaume; Ouèrmi Lucienne; Munga Stephen; Obor David; Bunker Aditi; Gunga Hanns-Christian; Belesova Kristine; Bärnighausen Till; Franke Jonas; Schwarz Maximilian; Maggioni Martina Anna; Sauerborn Rainer; </v>
-      </c>
-      <c r="H30" t="str">
         <v>2025</v>
-      </c>
-      <c r="I30" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="31">
@@ -1286,19 +926,7 @@
         <v>Deep Learning-Based Plant Phenotyping Framework: Analysis of Crop Life Cycle Data for Indian Farmers to Develop a Smart Agri-Field Management System</v>
       </c>
       <c r="E31" t="str">
-        <v>Lecture Notes in Networks and Systems</v>
-      </c>
-      <c r="F31" t="str">
-        <v/>
-      </c>
-      <c r="G31" t="str">
-        <v xml:space="preserve">Basak Sayanti; Saha Sarmistha; Halder Abinash; Hati Anirban Jyoti; Banerjee Bhaskar; Krishnamurthy V; </v>
-      </c>
-      <c r="H31" t="str">
         <v>2023</v>
-      </c>
-      <c r="I31" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="32">
@@ -1315,19 +943,7 @@
         <v>Perceptions and attitudes towards climate change in fishing communities of the Sudd Wetlands, South Sudan</v>
       </c>
       <c r="E32" t="str">
-        <v>Regional Environmental Change</v>
-      </c>
-      <c r="F32" t="str">
-        <v/>
-      </c>
-      <c r="G32" t="str">
-        <v xml:space="preserve">Benansio John Sebit; Funk Stephan Michael; Lino John Ladu; Balli Johnson Jiribi; Dante John Ohitai; Dendi Daniele; Fa Julia E; Luiselli Luca; </v>
-      </c>
-      <c r="H32" t="str">
         <v>2022</v>
-      </c>
-      <c r="I32" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="33">
@@ -1344,19 +960,7 @@
         <v>Micro-Investment by Tanzanian Smallholders’ in Drip Irrigation Kits for Vegetable Production to Improve Livelihoods: Lessons Learned and a Way Forward</v>
       </c>
       <c r="E33" t="str">
-        <v>Agriculture Switzerland</v>
-      </c>
-      <c r="F33" t="str">
-        <v/>
-      </c>
-      <c r="G33" t="str">
-        <v xml:space="preserve">Bhatti Muhammad Azher; Godfrey Sosheel Solomon; Divon Shai André; Aamodt Julie Therese; Øystese Siv; Wynn Peter C; Eik Lars Olav; Fjeld-Solberg Øivind; </v>
-      </c>
-      <c r="H33" t="str">
         <v>2022</v>
-      </c>
-      <c r="I33" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="34">
@@ -1373,19 +977,7 @@
         <v>Salinity patterns in irrigation systems, a threat to be demystified, a constraint to be managed: Field evidence from Algeria and Tunisia</v>
       </c>
       <c r="E34" t="str">
-        <v>Irrigation and Drainage</v>
-      </c>
-      <c r="F34" t="str">
-        <v/>
-      </c>
-      <c r="G34" t="str">
-        <v xml:space="preserve">Bouarfa S; Marlet S; Douaoui A; Hartani T; Mekki I; Ghazouani W; Aissa I Ben; Vincent B; Hassani F; Kuper M; </v>
-      </c>
-      <c r="H34" t="str">
         <v>2009</v>
-      </c>
-      <c r="I34" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="35">
@@ -1402,19 +994,7 @@
         <v>Burial societies in rural ethiopia</v>
       </c>
       <c r="E35" t="str">
-        <v>Collective Action and Property Rights for Poverty Reduction Insights from Africa and Asia</v>
-      </c>
-      <c r="F35" t="str">
-        <v/>
-      </c>
-      <c r="G35" t="str">
-        <v/>
-      </c>
-      <c r="H35" t="str">
         <v>2012</v>
-      </c>
-      <c r="I35" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="36">
@@ -1431,19 +1011,7 @@
         <v>Assessment of Prioritized Climate Smart Agricultural Practices and Technologies of Household Farmers in Southeast, Nigeria</v>
       </c>
       <c r="E36" t="str">
-        <v>Universal Journal of Agricultural Research</v>
-      </c>
-      <c r="F36" t="str">
-        <v/>
-      </c>
-      <c r="G36" t="str">
-        <v xml:space="preserve">C O; Igberi; E E; Osuji; N E; Odo; C C; Ibekwe; C S; Onyemauwa; H O; Obi; K C; Obike; I O; Obasi; A C; Ifejimalu; F E; Ebe; O B; Ibeagwa; I C; Chinaka; C P O; Emeka; J E; Orji; S Ibrahim-Olesin; </v>
-      </c>
-      <c r="H36" t="str">
         <v>2022</v>
-      </c>
-      <c r="I36" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="37">
@@ -1460,19 +1028,7 @@
         <v>Genotype-by-gestational thermal environment interaction and its impact on the future performance of tropical composite beef cattle offspring</v>
       </c>
       <c r="E37" t="str">
-        <v>Journal of Animal Science</v>
-      </c>
-      <c r="F37" t="str">
-        <v/>
-      </c>
-      <c r="G37" t="str">
-        <v xml:space="preserve">Cardoso Matheus Gomes Rodrigues; Bignardi Annaiza Braga; Pereira Rodrigo Junqueira; Eler Joanir Pereira; Ferraz José Bento Sterman; Brito Luiz Fernando; Santana Mário Luiz; </v>
-      </c>
-      <c r="H37" t="str">
         <v>2024</v>
-      </c>
-      <c r="I37" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="38">
@@ -1489,19 +1045,7 @@
         <v>Unintended effects of technology on climate change adaptation: An historical analysis of water conflicts below Andean Glaciers</v>
       </c>
       <c r="E38" t="str">
-        <v>Journal of Historical Geography</v>
-      </c>
-      <c r="F38" t="str">
-        <v/>
-      </c>
-      <c r="G38" t="str">
-        <v xml:space="preserve">Carey Mark; French Adam; O’Brien Elliott; </v>
-      </c>
-      <c r="H38" t="str">
         <v>2012</v>
-      </c>
-      <c r="I38" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="39">
@@ -1518,19 +1062,7 @@
         <v>Climate Change, Food Sovereignty, and Ancestral Farming Technologies in the Andes</v>
       </c>
       <c r="E39" t="str">
-        <v>Current Developments in Nutrition</v>
-      </c>
-      <c r="F39" t="str">
-        <v/>
-      </c>
-      <c r="G39" t="str">
-        <v xml:space="preserve">Carrasco-Torrontegui Amaya; Gallegos-Riofrío Carlos Andres; Delgado-Espinoza Florencio; Swanson Mark; </v>
-      </c>
-      <c r="H39" t="str">
         <v>2021</v>
-      </c>
-      <c r="I39" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="40">
@@ -1547,19 +1079,7 @@
         <v>Cases of Climate-Smart Agriculture in Southeast Asian highlands: Implications for ecosystem conservation and sustainability</v>
       </c>
       <c r="E40" t="str">
-        <v>Agriculture and Natural Resources</v>
-      </c>
-      <c r="F40" t="str">
-        <v/>
-      </c>
-      <c r="G40" t="str">
-        <v/>
-      </c>
-      <c r="H40" t="str">
         <v>2022</v>
-      </c>
-      <c r="I40" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="41">
@@ -1576,19 +1096,7 @@
         <v>Local food system resilience in the context of shocks and crises: vulnerabilities and responses of agroecology-based farmers in Peru, Germany, and the United States</v>
       </c>
       <c r="E41" t="str">
-        <v>Agroecology and Sustainable Food Systems</v>
-      </c>
-      <c r="F41" t="str">
-        <v/>
-      </c>
-      <c r="G41" t="str">
-        <v xml:space="preserve">Chavez-Miguel Giovanna; Hämmerle Janika; González Antonio; Canetti Chiara; Gleich Pia; Halfast Rebecca Lynn; Feuchter Moritz; Buszydlo Dominika; Schwarz Laura; Scheepstra Imke; de Haan Stef; Ccanto Raul; Sieber Stefan; Bonatti Michelle; </v>
-      </c>
-      <c r="H41" t="str">
         <v>2024</v>
-      </c>
-      <c r="I41" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="42">
@@ -1605,19 +1113,7 @@
         <v>Impact of seasonal hydrological variation on tropical fish assemblages: abrupt shift following an extreme flood event</v>
       </c>
       <c r="E42" t="str">
-        <v>Ecosphere</v>
-      </c>
-      <c r="F42" t="str">
-        <v/>
-      </c>
-      <c r="G42" t="str">
-        <v xml:space="preserve">Chea Ratha; Pool Thomas K; Chevalier Mathieu; Ngor Pengbun; So Nam; Winemiller Kirk O; Lek Sovan; Grenouillet Gaël; </v>
-      </c>
-      <c r="H42" t="str">
         <v>2020</v>
-      </c>
-      <c r="I42" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="43">
@@ -1634,19 +1130,7 @@
         <v>Microplastic transport and ecological risk in coastal intruded aquifers based on a coupled seawater intrusion and microplastic risk assessment model</v>
       </c>
       <c r="E43" t="str">
-        <v>Journal of Hazardous Materials</v>
-      </c>
-      <c r="F43" t="str">
-        <v/>
-      </c>
-      <c r="G43" t="str">
-        <v xml:space="preserve">Chen Guangquan; Zou Yinqiao; Xiong Guiyao; Wang Yancheng; Zhao Wenqing; Xu Xingyong; Zhu Xiaobin; Wu Jichun; Song Fan; Yu Hongjun; </v>
-      </c>
-      <c r="H43" t="str">
         <v>2024</v>
-      </c>
-      <c r="I43" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="44">
@@ -1663,19 +1147,7 @@
         <v>Enhancing Farmer Resilience Through Agricultural Insurance: Evidence from Jiangsu, China</v>
       </c>
       <c r="E44" t="str">
-        <v>Agriculture Switzerland</v>
-      </c>
-      <c r="F44" t="str">
-        <v/>
-      </c>
-      <c r="G44" t="str">
-        <v xml:space="preserve">Chen Xinru; Jiang Yuan; Wang Tianwei; Zhou Kexuan; Liu Jiayi; Ben Huirong; Wang Weidong; </v>
-      </c>
-      <c r="H44" t="str">
         <v>2025</v>
-      </c>
-      <c r="I44" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="45">
@@ -1692,19 +1164,7 @@
         <v>Consequences of climate change impacts and incidences of extreme weather events in relation to crop production in Bhutan</v>
       </c>
       <c r="E45" t="str">
-        <v>Sustainability Switzerland</v>
-      </c>
-      <c r="F45" t="str">
-        <v/>
-      </c>
-      <c r="G45" t="str">
-        <v xml:space="preserve">Chhogyel Ngawang; Kumar Lalit; Bajgai Yadunath; </v>
-      </c>
-      <c r="H45" t="str">
         <v>2020</v>
-      </c>
-      <c r="I45" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="46">
@@ -1721,19 +1181,7 @@
         <v>Impacts of social capital on climate change adaptations of banana farmers in Southern China</v>
       </c>
       <c r="E46" t="str">
-        <v>Environment Development and Sustainability</v>
-      </c>
-      <c r="F46" t="str">
-        <v/>
-      </c>
-      <c r="G46" t="str">
-        <v xml:space="preserve">Cishahayo Laurent; Zhu Yueji; Zhang Cheng; Wang Fang; </v>
-      </c>
-      <c r="H46" t="str">
         <v>2024</v>
-      </c>
-      <c r="I46" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="47">
@@ -1750,19 +1198,7 @@
         <v>Climatic risks and the livelihoods of cattle production families in the Costa Chica, Mexico</v>
       </c>
       <c r="E47" t="str">
-        <v>Tropical and Subtropical Agroecosystems</v>
-      </c>
-      <c r="F47" t="str">
-        <v/>
-      </c>
-      <c r="G47" t="str">
-        <v/>
-      </c>
-      <c r="H47" t="str">
         <v>2019</v>
-      </c>
-      <c r="I47" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="48">
@@ -1779,19 +1215,7 @@
         <v>Capacity building helps pastoral women transform impoverished communities in Ethiopia</v>
       </c>
       <c r="E48" t="str">
-        <v>Science</v>
-      </c>
-      <c r="F48" t="str">
-        <v/>
-      </c>
-      <c r="G48" t="str">
-        <v xml:space="preserve">Coppock D Layne; Desta Solomon; Tezera Seyoum; Gebru Getachew; </v>
-      </c>
-      <c r="H48" t="str">
         <v>2011</v>
-      </c>
-      <c r="I48" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="49">
@@ -1808,19 +1232,7 @@
         <v>Cropping systems: Applications, management and impact</v>
       </c>
       <c r="E49" t="str">
-        <v>Cropping Systems Applications Management and Impact</v>
-      </c>
-      <c r="F49" t="str">
-        <v/>
-      </c>
-      <c r="G49" t="str">
-        <v/>
-      </c>
-      <c r="H49" t="str">
         <v>2016</v>
-      </c>
-      <c r="I49" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="50">
@@ -1837,19 +1249,7 @@
         <v>Constructing A Climate-Smart readiness index for smallholder farmers: The case of prioritized bundles of climate information services and climate smart agriculture in Ghana</v>
       </c>
       <c r="E50" t="str">
-        <v>Climate Services</v>
-      </c>
-      <c r="F50" t="str">
-        <v/>
-      </c>
-      <c r="G50" t="str">
-        <v xml:space="preserve">Damba Osman Tahidu; Ageyo Collins Odhiambo; Kizito Fred; Mponela Powell; Yeboah Stephen; Clottey Victor Attuquaye; Oppong-Mensah Birgitta Adoma; Bayala Jules; Obeng Adomaa; Faustina; Dalaa Mustapha Alasan; Martey Francisca; Huyer Sophia; Zougmore Robert; Tepa-Yotto Ghislain; Tamò Manuele; </v>
-      </c>
-      <c r="H50" t="str">
         <v>2024</v>
-      </c>
-      <c r="I50" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="51">
@@ -1866,19 +1266,7 @@
         <v>Population genomics of the peripheral freshwater fish Polynemus melanochir (Perciformes, Polynemidae) in a changing Mekong Delta</v>
       </c>
       <c r="E51" t="str">
-        <v>Conservation Genetics</v>
-      </c>
-      <c r="F51" t="str">
-        <v/>
-      </c>
-      <c r="G51" t="str">
-        <v xml:space="preserve">Dang B T; Vu Q H. D; Biesack E E; Doan T V; Truong O T; Tran T L; Ackiss A S; Stockwell B L; Carpenter K E; </v>
-      </c>
-      <c r="H51" t="str">
         <v>2019</v>
-      </c>
-      <c r="I51" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="52">
@@ -1895,19 +1283,7 @@
         <v>Socio-economic vulnerability- climate resilience nexus in a few selected villages of Gosaba and Hingalganj CD Block of Sundarban, India</v>
       </c>
       <c r="E52" t="str">
-        <v>SN Social Sciences</v>
-      </c>
-      <c r="F52" t="str">
-        <v/>
-      </c>
-      <c r="G52" t="str">
-        <v xml:space="preserve">Das Semanti; Das Chandan Surabhi; </v>
-      </c>
-      <c r="H52" t="str">
         <v>2026</v>
-      </c>
-      <c r="I52" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="53">
@@ -1924,19 +1300,7 @@
         <v>The saga of community learning: Mariculture and the Bolinao experience</v>
       </c>
       <c r="E53" t="str">
-        <v>Aquatic Ecosystem Health and Management</v>
-      </c>
-      <c r="F53" t="str">
-        <v/>
-      </c>
-      <c r="G53" t="str">
-        <v xml:space="preserve">David Laura T; Pastor-Rengel Davelyn; Talaue-McManus Liana; Magdaong Evangeline; Salalila-Aruelo Rose; Bangi Helen Grace; San Diego-McGlone; Maria Lourdes; Villanoy Cesar; Cordero-Bailey Kristina; </v>
-      </c>
-      <c r="H53" t="str">
         <v>2014</v>
-      </c>
-      <c r="I53" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="54">
@@ -1953,19 +1317,7 @@
         <v>Development of sorghum for bio-energy: A view from the stakeholders and priorities for breeding dual purpose varieties</v>
       </c>
       <c r="E54" t="str">
-        <v>African Journal of Agricultural Research</v>
-      </c>
-      <c r="F54" t="str">
-        <v/>
-      </c>
-      <c r="G54" t="str">
-        <v/>
-      </c>
-      <c r="H54" t="str">
         <v>2011</v>
-      </c>
-      <c r="I54" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="55">
@@ -1982,19 +1334,7 @@
         <v>Thirty years of water management research for rice in sub-Saharan Africa: Achievement and perspectives</v>
       </c>
       <c r="E55" t="str">
-        <v>Field Crops Research</v>
-      </c>
-      <c r="F55" t="str">
-        <v/>
-      </c>
-      <c r="G55" t="str">
-        <v xml:space="preserve">Dossou-Yovo Elliott Ronald; Devkota Krishna Prasad; Akpoti Komlavi; Danvi Alexandre; Duku Confidence; Zwart Sander J; </v>
-      </c>
-      <c r="H55" t="str">
         <v>2022</v>
-      </c>
-      <c r="I55" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="56">
@@ -2011,19 +1351,7 @@
         <v>Factors shaping plant diversity in traditional agroforestry system of dominant ethnic communities of upper Brahmaputra valley regions of Northeast India</v>
       </c>
       <c r="E56" t="str">
-        <v>Agroforestry Systems</v>
-      </c>
-      <c r="F56" t="str">
-        <v/>
-      </c>
-      <c r="G56" t="str">
-        <v xml:space="preserve">Dutta Madhusmita; Deb Panna; Das Ashesh Kumar; </v>
-      </c>
-      <c r="H56" t="str">
         <v>2023</v>
-      </c>
-      <c r="I56" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="57">
@@ -2040,19 +1368,7 @@
         <v>Economic-engineering optimization to assess climate change impacts on agriculture in morocco</v>
       </c>
       <c r="E57" t="str">
-        <v>International Journal of Applied Engineering Research</v>
-      </c>
-      <c r="F57" t="str">
-        <v/>
-      </c>
-      <c r="G57" t="str">
-        <v/>
-      </c>
-      <c r="H57" t="str">
         <v>2017</v>
-      </c>
-      <c r="I57" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="58">
@@ -2069,19 +1385,7 @@
         <v>Innovation without participation? Moroccan farmers' perspectives on Haouz Mejjat aquifer contract</v>
       </c>
       <c r="E58" t="str">
-        <v>Groundwater for Sustainable Development</v>
-      </c>
-      <c r="F58" t="str">
-        <v/>
-      </c>
-      <c r="G58" t="str">
-        <v xml:space="preserve">El Mansoum Rachida; Chfadi Tarik; </v>
-      </c>
-      <c r="H58" t="str">
         <v>2025</v>
-      </c>
-      <c r="I58" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="59">
@@ -2098,19 +1402,7 @@
         <v>Factors Influencing the Acceptance and Use of the Internet of Things (IoT) by Thai Farmers</v>
       </c>
       <c r="E59" t="str">
-        <v>Thammasat Review</v>
-      </c>
-      <c r="F59" t="str">
-        <v/>
-      </c>
-      <c r="G59" t="str">
-        <v/>
-      </c>
-      <c r="H59" t="str">
         <v>2025</v>
-      </c>
-      <c r="I59" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="60">
@@ -2127,19 +1419,7 @@
         <v>Seascape connectivity of European anchovy in the Central Mediterranean Sea revealed by weighted Lagrangian backtracking and bio-energetic modelling</v>
       </c>
       <c r="E60" t="str">
-        <v>Scientific Reports</v>
-      </c>
-      <c r="F60" t="str">
-        <v/>
-      </c>
-      <c r="G60" t="str">
-        <v xml:space="preserve">Falcini Federico; Corrado Raffaele; Torri Marco; Mangano Maria Cristina; Zarrad Rafik; Di Cintio Antonio; Palatella Luigi; Jarboui Othman; Missaoui Hechmi; Cuttitta Angela; Patti Bernardo; Santoleri Rosalia; Sarà Gianluca; Lacorata Guglielmo; </v>
-      </c>
-      <c r="H60" t="str">
         <v>2020</v>
-      </c>
-      <c r="I60" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="61">
@@ -2156,19 +1436,7 @@
         <v>From Flood Mitigation to Environmental and Socioeconomic Disruption: A Case Study of the Langue de Barbarie Sand Spit Breach</v>
       </c>
       <c r="E61" t="str">
-        <v>Hydrology</v>
-      </c>
-      <c r="F61" t="str">
-        <v/>
-      </c>
-      <c r="G61" t="str">
-        <v xml:space="preserve">Fall Souleymane; </v>
-      </c>
-      <c r="H61" t="str">
         <v>2025</v>
-      </c>
-      <c r="I61" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="62">
@@ -2185,19 +1453,7 @@
         <v>FARMING ADAPTATION IN THE WESTERN SUDANESE SAVANNAH: LESSONS LEARNT AND CHALLENGES AHEAD</v>
       </c>
       <c r="E62" t="str">
-        <v>Advancing Climate Change Research in West Africa Trends Impacts Vulnerability Resilience Adaptation and Sustainability Issues</v>
-      </c>
-      <c r="F62" t="str">
-        <v/>
-      </c>
-      <c r="G62" t="str">
-        <v/>
-      </c>
-      <c r="H62" t="str">
         <v>2019</v>
-      </c>
-      <c r="I62" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="63">
@@ -2214,19 +1470,7 @@
         <v>Hydrogeochemical characterization and suitability of water for irrigation in new and old reservoirs in northern Espirito Santo, Brazil</v>
       </c>
       <c r="E63" t="str">
-        <v>Environment Development and Sustainability</v>
-      </c>
-      <c r="F63" t="str">
-        <v/>
-      </c>
-      <c r="G63" t="str">
-        <v xml:space="preserve">Favero Daiane; Cotta Aloísio José Bueno; Bonomo Robson; Rodrigues Murilo Brazzali; </v>
-      </c>
-      <c r="H63" t="str">
         <v>2022</v>
-      </c>
-      <c r="I63" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="64">
@@ -2243,19 +1487,7 @@
         <v>Water Saving and Environmental Issues in the Hetao Irrigation District, the Yellow River Basin: Development Perspective Analysis</v>
       </c>
       <c r="E64" t="str">
-        <v>Agronomy</v>
-      </c>
-      <c r="F64" t="str">
-        <v/>
-      </c>
-      <c r="G64" t="str">
-        <v xml:space="preserve">Feng Zhuangzhuang; Miao Qingfeng; Shi Haibin; Gonçalves José Manuel; Li Ruiping; </v>
-      </c>
-      <c r="H64" t="str">
         <v>2025</v>
-      </c>
-      <c r="I64" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="65">
@@ -2272,19 +1504,7 @@
         <v>Warm winters challenge the cultivation of temperate species in South America—a spatial analysis of chill accumulation</v>
       </c>
       <c r="E65" t="str">
-        <v>Climatic Change</v>
-      </c>
-      <c r="F65" t="str">
-        <v/>
-      </c>
-      <c r="G65" t="str">
-        <v xml:space="preserve">Fernandez Eduardo; Caspersen Lars; Illert Ilja; Luedeling Eike; </v>
-      </c>
-      <c r="H65" t="str">
         <v>2021</v>
-      </c>
-      <c r="I65" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="66">
@@ -2301,19 +1521,7 @@
         <v>Climate change, water availability, and the burden of rural women's triple role in Muyuka, Cameroon</v>
       </c>
       <c r="E66" t="str">
-        <v>Global Environmental Change</v>
-      </c>
-      <c r="F66" t="str">
-        <v/>
-      </c>
-      <c r="G66" t="str">
-        <v xml:space="preserve">Fonjong Lotsmart; Zama Regina Ndip; </v>
-      </c>
-      <c r="H66" t="str">
         <v>2023</v>
-      </c>
-      <c r="I66" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="67">
@@ -2330,19 +1538,7 @@
         <v>Using temporal NDVI/MODIS profiles for inferences on the crop soybean calendar</v>
       </c>
       <c r="E67" t="str">
-        <v>Bragantia</v>
-      </c>
-      <c r="F67" t="str">
-        <v/>
-      </c>
-      <c r="G67" t="str">
-        <v xml:space="preserve">Fontana Denise Cybis; Pinto Daniele Gutterres; Junges Amanda Heemann; Bremm Carolina; </v>
-      </c>
-      <c r="H67" t="str">
         <v>2015</v>
-      </c>
-      <c r="I67" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="68">
@@ -2359,19 +1555,7 @@
         <v>Comparing carbon offsets and livelihood benefits in a long-term reforestation project: Agroforestry versus native timber versus enrichment planting</v>
       </c>
       <c r="E68" t="str">
-        <v>Ecological Solutions and Evidence</v>
-      </c>
-      <c r="F68" t="str">
-        <v/>
-      </c>
-      <c r="G68" t="str">
-        <v xml:space="preserve">Forgues Katia; Carignan Marie‐Claude; Marchena Brais; Mancilla Lady; Pacheco Cristian; Pacheco Ortega; Elionel; Guainora Ariosto; Potvin Catherine; </v>
-      </c>
-      <c r="H68" t="str">
         <v>2024</v>
-      </c>
-      <c r="I68" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="69">
@@ -2388,19 +1572,7 @@
         <v>Spatial–temporal variations of oceanographic parameters in the Zhoushan sea area of the East China Sea based on remote sensing datasets</v>
       </c>
       <c r="E69" t="str">
-        <v>Regional Studies in Marine Science</v>
-      </c>
-      <c r="F69" t="str">
-        <v/>
-      </c>
-      <c r="G69" t="str">
-        <v xml:space="preserve">Fu Jiaoqi; Chen Chao; Chu Yanli; </v>
-      </c>
-      <c r="H69" t="str">
         <v>2019</v>
-      </c>
-      <c r="I69" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="70">
@@ -2417,19 +1589,7 @@
         <v>Toward the development of a weather index insurance for rice farmers in the coastal region of Myanmar</v>
       </c>
       <c r="E70" t="str">
-        <v>Paddy and Water Environment</v>
-      </c>
-      <c r="F70" t="str">
-        <v/>
-      </c>
-      <c r="G70" t="str">
-        <v xml:space="preserve">Furuya Jun; Omori Keisuke; Aizaki Hideo; </v>
-      </c>
-      <c r="H70" t="str">
         <v>2021</v>
-      </c>
-      <c r="I70" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="71">
@@ -2446,19 +1606,7 @@
         <v>Tweaking Pakistani Punjab rice-wheat management to maximize productivity within nitrate leaching limits</v>
       </c>
       <c r="E71" t="str">
-        <v>Field Crops Research</v>
-      </c>
-      <c r="F71" t="str">
-        <v/>
-      </c>
-      <c r="G71" t="str">
-        <v xml:space="preserve">Gaydon Donald S; Khaliq Tasneem; Ahmad Mobin-ud-Din; Cheema M J.M; Gull Umair; </v>
-      </c>
-      <c r="H71" t="str">
         <v>2021</v>
-      </c>
-      <c r="I71" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="72">
@@ -2475,19 +1623,7 @@
         <v>Gender differences in smallholder farmers’ adoption of crop diversification: Evidence from Shaanxi Plain, China</v>
       </c>
       <c r="E72" t="str">
-        <v>Climate Risk Management</v>
-      </c>
-      <c r="F72" t="str">
-        <v/>
-      </c>
-      <c r="G72" t="str">
-        <v xml:space="preserve">Ge Yuhang; Fan Liangxin; Li Yingbin; Guo Jin; Niu Haipeng; </v>
-      </c>
-      <c r="H72" t="str">
         <v>2023</v>
-      </c>
-      <c r="I72" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="73">
@@ -2504,19 +1640,7 @@
         <v>Environmental and social impacts of women’s argan oil production in Morocco</v>
       </c>
       <c r="E73" t="str">
-        <v>International Journal of Life Cycle Assessment</v>
-      </c>
-      <c r="F73" t="str">
-        <v/>
-      </c>
-      <c r="G73" t="str">
-        <v xml:space="preserve">Gebrai Yoel; Naughton Colleen C; Sánchez Kimberly D; Bargach Jamila; Deubel Tara F; </v>
-      </c>
-      <c r="H73" t="str">
         <v>2025</v>
-      </c>
-      <c r="I73" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="74">
@@ -2533,19 +1657,7 @@
         <v>Investigation of the response of sweet cherries to root mycorrhisation with biologics for sustainable horticulture development</v>
       </c>
       <c r="E74" t="str">
-        <v>Scientific Horizons</v>
-      </c>
-      <c r="F74" t="str">
-        <v/>
-      </c>
-      <c r="G74" t="str">
-        <v xml:space="preserve">Gerasko Tetyana; Tymoshchuk Tetiana; Sayuk Oleksandr; Rudenko Yurii; Mrynskyi Іvan; </v>
-      </c>
-      <c r="H74" t="str">
         <v>2023</v>
-      </c>
-      <c r="I74" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="75">
@@ -2562,19 +1674,7 @@
         <v>Agroforestry systems in Nepal: Enhancing food security and rural livelihoods – a comprehensive review</v>
       </c>
       <c r="E75" t="str">
-        <v>Food and Energy Security</v>
-      </c>
-      <c r="F75" t="str">
-        <v/>
-      </c>
-      <c r="G75" t="str">
-        <v xml:space="preserve">Ghimire Manisha; Khanal Ashish; Bhatt Deepa; Dahal DhirajDatta; Giri Suja; </v>
-      </c>
-      <c r="H75" t="str">
         <v>2024</v>
-      </c>
-      <c r="I75" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="76">
@@ -2591,19 +1691,7 @@
         <v>Biological Features of Neoseiulus californicus (Acari: Phytoseiidae) Feeding on Schizotetranychus oryzae (Acari: Tetranychidae) Kept on Rice Leaves</v>
       </c>
       <c r="E76" t="str">
-        <v>Journal of Economic Entomology</v>
-      </c>
-      <c r="F76" t="str">
-        <v/>
-      </c>
-      <c r="G76" t="str">
-        <v xml:space="preserve">Gonçalves Dinarte; Cunha da Uemerson Silva; Rode Priscila de Andrade; Toldi Maicon; Ferla Noeli Juarez; </v>
-      </c>
-      <c r="H76" t="str">
         <v>2019</v>
-      </c>
-      <c r="I76" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="77">
@@ -2620,19 +1708,7 @@
         <v>Too much, too soon? Early-maturing maize varieties as drought escape strategy in Malawi</v>
       </c>
       <c r="E77" t="str">
-        <v>Food Policy</v>
-      </c>
-      <c r="F77" t="str">
-        <v/>
-      </c>
-      <c r="G77" t="str">
-        <v xml:space="preserve">Grewer Uwe; Kim Dong-Hyuk; Waha Katharina; </v>
-      </c>
-      <c r="H77" t="str">
         <v>2024</v>
-      </c>
-      <c r="I77" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="78">
@@ -2649,19 +1725,7 @@
         <v>Old abandoned terraces surveying and restoration as a contribution to the adaptive forest landscape restoration in Lebanon</v>
       </c>
       <c r="E78" t="str">
-        <v>Acta Horticulturae</v>
-      </c>
-      <c r="F78" t="str">
-        <v/>
-      </c>
-      <c r="G78" t="str">
-        <v xml:space="preserve">Hani N; Regato P; Pagliani M; Khaddazh M; Vernyuk Y I; Sarkis L; BuHussein R; Buwadi M; Dokukin P; </v>
-      </c>
-      <c r="H78" t="str">
         <v>2021</v>
-      </c>
-      <c r="I78" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="79">
@@ -2678,19 +1742,7 @@
         <v>Adoption of climate-smart agriculture practices and differentiated nutritional outcome among rural households: a case of Punjab province, Pakistan</v>
       </c>
       <c r="E79" t="str">
-        <v>Food Security</v>
-      </c>
-      <c r="F79" t="str">
-        <v/>
-      </c>
-      <c r="G79" t="str">
-        <v xml:space="preserve">Haq Shamsheer ul; Boz Ismet; Shahbaz Pomi; </v>
-      </c>
-      <c r="H79" t="str">
         <v>2021</v>
-      </c>
-      <c r="I79" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="80">
@@ -2707,19 +1759,7 @@
         <v>Extreme climate events increase risk of global food insecurity and adaptation needs</v>
       </c>
       <c r="E80" t="str">
-        <v>Nature Food</v>
-      </c>
-      <c r="F80" t="str">
-        <v/>
-      </c>
-      <c r="G80" t="str">
-        <v xml:space="preserve">Hasegawa Tomoko; Sakurai Gen; Fujimori Shinichiro; Takahashi Kiyoshi; Hijioka Yasuaki; Masui Toshihiko; </v>
-      </c>
-      <c r="H80" t="str">
         <v>2021</v>
-      </c>
-      <c r="I80" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="81">
@@ -2736,19 +1776,7 @@
         <v>The first nation-wide assessment identifies valuable blue‑carbon seagrass habitat in Indonesia is in moderate condition</v>
       </c>
       <c r="E81" t="str">
-        <v>Science of the Total Environment</v>
-      </c>
-      <c r="F81" t="str">
-        <v/>
-      </c>
-      <c r="G81" t="str">
-        <v xml:space="preserve">Hernawan Udhi E; Rahmawati Susi; Ambo-Rappe Rohani; Sjafrie Nurul D.M; Hadiyanto Hadiyanto; Yusup Deny S; Nugraha Aditya H; La Nafie Yayu A; Adi Wahyu; Prayudha Bayu; Irawan Andri; Rahayu Yusmiana P; Ningsih Ermi; Riniatsih Ita; Supriyadi Indarto H; McMahon Kathryn; </v>
-      </c>
-      <c r="H81" t="str">
         <v>2021</v>
-      </c>
-      <c r="I81" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="82">
@@ -2765,19 +1793,7 @@
         <v>Adaptation to climate change in Uganda: Evidence from micro level data</v>
       </c>
       <c r="E82" t="str">
-        <v>Global Environmental Change</v>
-      </c>
-      <c r="F82" t="str">
-        <v/>
-      </c>
-      <c r="G82" t="str">
-        <v xml:space="preserve">Hisali Eria; Birungi Patrick; Buyinza Faisal; </v>
-      </c>
-      <c r="H82" t="str">
         <v>2011</v>
-      </c>
-      <c r="I82" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="83">
@@ -2794,19 +1810,7 @@
         <v>Assessing the vulnerability of small-scale fishery communities in the estuarine areas of Central Vietnam in the context of increasing climate risks</v>
       </c>
       <c r="E83" t="str">
-        <v>Ocean and Coastal Management</v>
-      </c>
-      <c r="F83" t="str">
-        <v/>
-      </c>
-      <c r="G83" t="str">
-        <v xml:space="preserve">Hoang Ha Dung; Momtaz Salim; Schreider Maria; </v>
-      </c>
-      <c r="H83" t="str">
         <v>2020</v>
-      </c>
-      <c r="I83" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="84">
@@ -2823,19 +1827,7 @@
         <v>Motivating factors of farmers’ adaptation behaviors to climate change in China: A meta-analysis</v>
       </c>
       <c r="E84" t="str">
-        <v>Journal of Environmental Management</v>
-      </c>
-      <c r="F84" t="str">
-        <v/>
-      </c>
-      <c r="G84" t="str">
-        <v xml:space="preserve">Huang Yingqian; Long Hualou; Jiang Yanfeng; Feng Dedong; Ma Zizhou; Mumtaz Faisal; </v>
-      </c>
-      <c r="H84" t="str">
         <v>2024</v>
-      </c>
-      <c r="I84" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="85">
@@ -2852,19 +1844,7 @@
         <v>Social practices of knowledge mobilization for sustainable food production: nutrition gardening and fish farming in the kolli hills of India</v>
       </c>
       <c r="E85" t="str">
-        <v>Food Security</v>
-      </c>
-      <c r="F85" t="str">
-        <v/>
-      </c>
-      <c r="G85" t="str">
-        <v xml:space="preserve">Hudson Suraya; Krogman Naomi; Beckie Mary; </v>
-      </c>
-      <c r="H85" t="str">
         <v>2016</v>
-      </c>
-      <c r="I85" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="86">
@@ -2881,19 +1861,7 @@
         <v>Impacts of climate change and variability on agriculture-experience from Europe and India</v>
       </c>
       <c r="E86" t="str">
-        <v>Journal of Agrometeorology</v>
-      </c>
-      <c r="F86" t="str">
-        <v/>
-      </c>
-      <c r="G86" t="str">
-        <v/>
-      </c>
-      <c r="H86" t="str">
         <v>2009</v>
-      </c>
-      <c r="I86" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="87">
@@ -2910,19 +1878,7 @@
         <v>In situ rain water harvesting techniques increase maize growth and grain yield in a semi-arid agro-ecology of Nyagatare, Rwanda</v>
       </c>
       <c r="E87" t="str">
-        <v>International Journal of Agriculture and Biology</v>
-      </c>
-      <c r="F87" t="str">
-        <v/>
-      </c>
-      <c r="G87" t="str">
-        <v/>
-      </c>
-      <c r="H87" t="str">
         <v>2014</v>
-      </c>
-      <c r="I87" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="88">
@@ -2939,19 +1895,7 @@
         <v>Integrating crop improvement with resource management to alleviate the effects of desertification under climate change scenarios</v>
       </c>
       <c r="E88" t="str">
-        <v>Annals of Arid Zone</v>
-      </c>
-      <c r="F88" t="str">
-        <v/>
-      </c>
-      <c r="G88" t="str">
-        <v/>
-      </c>
-      <c r="H88" t="str">
         <v>2011</v>
-      </c>
-      <c r="I88" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="89">
@@ -2968,19 +1912,7 @@
         <v>Innovative Regenerative Technologies for Enhancing Resilience in Salinity-Stressed Rice Fields Along the Indonesian Coast: Promoting Net-Zero Farming Practices to Adapt to Climate Change</v>
       </c>
       <c r="E89" t="str">
-        <v>Journal of Sustainable Agriculture and Environment</v>
-      </c>
-      <c r="F89" t="str">
-        <v/>
-      </c>
-      <c r="G89" t="str">
-        <v xml:space="preserve">Irwandhi Irwandhi; Khumairah Fiqriah Hanum; Sofyan Emma Trinurani; Ukit Ukit; Satria Rievansyah Eka; Salsabilla Annisya; Sauri Muhamad Sopyan; Simarmata Tualar; </v>
-      </c>
-      <c r="H89" t="str">
         <v>2024</v>
-      </c>
-      <c r="I89" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="90">
@@ -2997,19 +1929,7 @@
         <v>Unravelling the complexities of wetland agriculture, climate change, and coping mechanisms: an integrative review using economics and satellite approaches</v>
       </c>
       <c r="E90" t="str">
-        <v>Environment Development and Sustainability</v>
-      </c>
-      <c r="F90" t="str">
-        <v/>
-      </c>
-      <c r="G90" t="str">
-        <v xml:space="preserve">Islam Md Monirul; </v>
-      </c>
-      <c r="H90" t="str">
         <v>2024</v>
-      </c>
-      <c r="I90" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="91">
@@ -3026,19 +1946,7 @@
         <v>Dynamic Evaluation and Risk Projection of Heat Exposure Based on Disaster Events for Single-Season Rice along the Middle and Lower Reaches of the Yangtze River, China</v>
       </c>
       <c r="E91" t="str">
-        <v>Agronomy</v>
-      </c>
-      <c r="F91" t="str">
-        <v/>
-      </c>
-      <c r="G91" t="str">
-        <v xml:space="preserve">Jiang Mengyuan; Huo Zhiguo; Zhang Lei; Zhang Fengyin; Li Meixuan; Mi Qianchuan; Kong Rui; </v>
-      </c>
-      <c r="H91" t="str">
         <v>2024</v>
-      </c>
-      <c r="I91" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="92">
@@ -3055,19 +1963,7 @@
         <v>Contextual vulnerability of rainfed crop-based farming communities in semi-arid Zimbabwe: A case of Chiredzi District</v>
       </c>
       <c r="E92" t="str">
-        <v>International Journal of Climate Change Strategies and Management</v>
-      </c>
-      <c r="F92" t="str">
-        <v/>
-      </c>
-      <c r="G92" t="str">
-        <v xml:space="preserve">Jiri Obert; Mafongoya Paramu L; Chivenge Pauline; </v>
-      </c>
-      <c r="H92" t="str">
         <v>2017</v>
-      </c>
-      <c r="I92" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="93">
@@ -3084,19 +1980,7 @@
         <v>A Comparative Study of the Impacts of Flooding on Food Security of Urban and Rural Households in Blantyre City and Chikwawa, Malawi</v>
       </c>
       <c r="E93" t="str">
-        <v>Sustainable Development Goals Series</v>
-      </c>
-      <c r="F93" t="str">
-        <v/>
-      </c>
-      <c r="G93" t="str">
-        <v xml:space="preserve">Joshua Miriam Dalitso Kalanda; Stathers Tanya; Chirwa Ruth Kalinga; Ngongondo Cosmo; Lamboll Richard; Monjerezi Maurice; Mwathunga Evance; Kasei Raymond; Chipungu Felistus Patience; Liwenga Emma Teresa; </v>
-      </c>
-      <c r="H93" t="str">
         <v>2021</v>
-      </c>
-      <c r="I93" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="94">
@@ -3113,19 +1997,7 @@
         <v>Temporal variability of ENSO effects on corn yield at the central region of Argentina</v>
       </c>
       <c r="E94" t="str">
-        <v>International Journal of Climatology</v>
-      </c>
-      <c r="F94" t="str">
-        <v/>
-      </c>
-      <c r="G94" t="str">
-        <v xml:space="preserve">Jozami Emiliano; Montero Bulacio; Enrique; Coronel Alejandra; </v>
-      </c>
-      <c r="H94" t="str">
         <v>2018</v>
-      </c>
-      <c r="I94" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="95">
@@ -3142,19 +2014,7 @@
         <v>Tree knowledge and livelihood activities in a changing environment: Views from smallholder farmers in Kosti, Sudan</v>
       </c>
       <c r="E95" t="str">
-        <v>Journal of Sustainable Forestry</v>
-      </c>
-      <c r="F95" t="str">
-        <v/>
-      </c>
-      <c r="G95" t="str">
-        <v xml:space="preserve">Kalame Fobissie B; Luukkanen Olavi; Elsiddig Elnour A; Glover Edinam K; </v>
-      </c>
-      <c r="H95" t="str">
         <v>2010</v>
-      </c>
-      <c r="I95" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="96">
@@ -3171,19 +2031,7 @@
         <v>Role of smallholder tea growers in carbon sink management</v>
       </c>
       <c r="E96" t="str">
-        <v>Current Science</v>
-      </c>
-      <c r="F96" t="str">
-        <v/>
-      </c>
-      <c r="G96" t="str">
-        <v xml:space="preserve">Kalita Rinku Moni; Das Ashesh Kumar; Nath Arun Jyoti; </v>
-      </c>
-      <c r="H96" t="str">
         <v>2019</v>
-      </c>
-      <c r="I96" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="97">
@@ -3200,19 +2048,7 @@
         <v>Impacts of agricultural water interventions on farm income: An example from the Kothapally watershed, India</v>
       </c>
       <c r="E97" t="str">
-        <v>Agricultural Systems</v>
-      </c>
-      <c r="F97" t="str">
-        <v/>
-      </c>
-      <c r="G97" t="str">
-        <v xml:space="preserve">Karlberg L; Garg K K; Barron J; Wani S P; </v>
-      </c>
-      <c r="H97" t="str">
         <v>2015</v>
-      </c>
-      <c r="I97" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="98">
@@ -3229,19 +2065,7 @@
         <v>Entering the Digital Research Age: Investigating the Effectiveness of Visual Digital Tools in Agricultural Research</v>
       </c>
       <c r="E98" t="str">
-        <v>Field Methods</v>
-      </c>
-      <c r="F98" t="str">
-        <v/>
-      </c>
-      <c r="G98" t="str">
-        <v xml:space="preserve">Kawerau Laura; Birkenberg Athena; Daum Thomas; Butele Cosmas Alfred; Birner Regina; </v>
-      </c>
-      <c r="H98" t="str">
         <v>2024</v>
-      </c>
-      <c r="I98" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="99">
@@ -3258,19 +2082,7 @@
         <v>Assessment of farmers’ local adaptation strategies to climate variability impacts in Hulbarag district Ethiopia</v>
       </c>
       <c r="E99" t="str">
-        <v>Discover Sustainability</v>
-      </c>
-      <c r="F99" t="str">
-        <v/>
-      </c>
-      <c r="G99" t="str">
-        <v xml:space="preserve">Kerebo Kelifa Ahmed; Bizuneh Yechale Kebede; Mekonnen Abren Gelaw; Mohammed Yimer; </v>
-      </c>
-      <c r="H99" t="str">
         <v>2025</v>
-      </c>
-      <c r="I99" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="100">
@@ -3287,19 +2099,7 @@
         <v>Agro-pastoralists’ determinants of adaptation to climate change</v>
       </c>
       <c r="E100" t="str">
-        <v>International Journal of Climate Change Strategies and Management</v>
-      </c>
-      <c r="F100" t="str">
-        <v/>
-      </c>
-      <c r="G100" t="str">
-        <v xml:space="preserve">Kgosikoma Keneilwe Ruth; Lekota Phatsimo Cotildah; Kgosikoma Olaotswe Ernest; </v>
-      </c>
-      <c r="H100" t="str">
         <v>2018</v>
-      </c>
-      <c r="I100" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="101">
@@ -3316,19 +2116,7 @@
         <v>Indigenous coping and adaptation strategies to climate change of local communities in Tanzania: a review</v>
       </c>
       <c r="E101" t="str">
-        <v>Climate and Development</v>
-      </c>
-      <c r="F101" t="str">
-        <v/>
-      </c>
-      <c r="G101" t="str">
-        <v xml:space="preserve">Kihila Jacob M; </v>
-      </c>
-      <c r="H101" t="str">
         <v>2018</v>
-      </c>
-      <c r="I101" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="102">
@@ -3345,19 +2133,7 @@
         <v>A meta-analysis of economic and environmental benefits of conservation agriculture in South Asia</v>
       </c>
       <c r="E102" t="str">
-        <v>Journal of Environmental Management</v>
-      </c>
-      <c r="F102" t="str">
-        <v/>
-      </c>
-      <c r="G102" t="str">
-        <v xml:space="preserve">Kiran Kumara; T M; Kandpal Ankita; Pal Suresh; </v>
-      </c>
-      <c r="H102" t="str">
         <v>2020</v>
-      </c>
-      <c r="I102" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="103">
@@ -3374,19 +2150,7 @@
         <v>Impact of adoption of heat-stress tolerant maize hybrid on yield and profitability: Evidence from Terai region of Nepal</v>
       </c>
       <c r="E103" t="str">
-        <v>Frontiers in Sustainable Food Systems</v>
-      </c>
-      <c r="F103" t="str">
-        <v/>
-      </c>
-      <c r="G103" t="str">
-        <v xml:space="preserve">Kulkarni Atul P; Tripathi Mahendra P; Gautam Damodar; Koirala Keshab B; Kandel Manoj; Regmi Dhruba; Sapkota Sudha; Zaidi Pervez Haider; </v>
-      </c>
-      <c r="H103" t="str">
         <v>2023</v>
-      </c>
-      <c r="I103" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="104">
@@ -3403,19 +2167,7 @@
         <v>Google Earth Engine-Based Identification of Flood Extent and Flood-Affected Paddy Rice Fields Using Sentinel-2 MSI and Sentinel-1 SAR Data in Bihar State, India</v>
       </c>
       <c r="E104" t="str">
-        <v>Journal of the Indian Society of Remote Sensing</v>
-      </c>
-      <c r="F104" t="str">
-        <v/>
-      </c>
-      <c r="G104" t="str">
-        <v xml:space="preserve">Kumar Himanshu; Karwariya Sateesh Kumar; Kumar Rohan; </v>
-      </c>
-      <c r="H104" t="str">
         <v>2022</v>
-      </c>
-      <c r="I104" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="105">
@@ -3432,19 +2184,7 @@
         <v>Social protection for transformative resilience: do programmes really address underlying causes of vulnerability of subsistence farmers to climate change?</v>
       </c>
       <c r="E105" t="str">
-        <v>Local Environment</v>
-      </c>
-      <c r="F105" t="str">
-        <v/>
-      </c>
-      <c r="G105" t="str">
-        <v xml:space="preserve">Kundo Hare Krisna; Spencer Rochelle; Brueckner Martin; Davis John K; </v>
-      </c>
-      <c r="H105" t="str">
         <v>2024</v>
-      </c>
-      <c r="I105" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="106">
@@ -3461,19 +2201,7 @@
         <v>Restoring Soil Organic Matter Content for Managing Soil Health in Africa’s Agroecoregions</v>
       </c>
       <c r="E106" t="str">
-        <v>Egyptian Journal of Soil Science</v>
-      </c>
-      <c r="F106" t="str">
-        <v/>
-      </c>
-      <c r="G106" t="str">
-        <v xml:space="preserve">Lal Rattan; </v>
-      </c>
-      <c r="H106" t="str">
         <v>2025</v>
-      </c>
-      <c r="I106" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="107">
@@ -3490,19 +2218,7 @@
         <v>Innovation in two contrasting value chains: Constraints and opportunities for adopting alternative crop production in the Vietnamese Mekong River Delta</v>
       </c>
       <c r="E107" t="str">
-        <v>Regional Sustainability</v>
-      </c>
-      <c r="F107" t="str">
-        <v/>
-      </c>
-      <c r="G107" t="str">
-        <v xml:space="preserve">Le Sang Thanh; Mao Nhu Huynh; Kristiansen Paul; Coleman Michael; </v>
-      </c>
-      <c r="H107" t="str">
         <v>2025</v>
-      </c>
-      <c r="I107" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="108">
@@ -3519,19 +2235,7 @@
         <v>Effects of fishery complementary photovoltaic power plant on near-surface meteorology and energy balance</v>
       </c>
       <c r="E108" t="str">
-        <v>Renewable Energy</v>
-      </c>
-      <c r="F108" t="str">
-        <v/>
-      </c>
-      <c r="G108" t="str">
-        <v xml:space="preserve">Li Peidu; Gao Xiaoqing; Li Zhenchao; Ye Tiange; Zhou Xiyin; </v>
-      </c>
-      <c r="H108" t="str">
         <v>2022</v>
-      </c>
-      <c r="I108" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="109">
@@ -3548,19 +2252,7 @@
         <v>Spatiotemporal variations in suitable areas for Japanese scallop aquaculture in the Dalian coastal area from 2003 to 2012</v>
       </c>
       <c r="E109" t="str">
-        <v>Aquaculture</v>
-      </c>
-      <c r="F109" t="str">
-        <v/>
-      </c>
-      <c r="G109" t="str">
-        <v xml:space="preserve">Liu Yang; Saitoh Sei-Ichi; Radiarta I Nyoman; Igarashi Hiromichi; Hirawake Toru; </v>
-      </c>
-      <c r="H109" t="str">
         <v>2014</v>
-      </c>
-      <c r="I109" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="110">
@@ -3577,19 +2269,7 @@
         <v>The role of local institutions in building smallholder farmers' adaptive capacity against climate change impacts in Bikita, Zimbabwe</v>
       </c>
       <c r="E110" t="str">
-        <v>Africa S Radicalisms and Conservatisms Pop Culture Environment Colonialism and Migration</v>
-      </c>
-      <c r="F110" t="str">
-        <v/>
-      </c>
-      <c r="G110" t="str">
-        <v xml:space="preserve">Mafongoya Owen; Mafongoya Paramu; Mudhara Maxwell; </v>
-      </c>
-      <c r="H110" t="str">
         <v>2022</v>
-      </c>
-      <c r="I110" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="111">
@@ -3606,19 +2286,7 @@
         <v>Farmers’ adaptation strategies to combat the impacts of climate change on grapevine production in Dodoma, Tanzania</v>
       </c>
       <c r="E111" t="str">
-        <v>East African Journal of Science Technology and Innovation</v>
-      </c>
-      <c r="F111" t="str">
-        <v/>
-      </c>
-      <c r="G111" t="str">
-        <v xml:space="preserve">MAHENGE F Y; </v>
-      </c>
-      <c r="H111" t="str">
         <v>2024</v>
-      </c>
-      <c r="I111" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="112">
@@ -3635,19 +2303,7 @@
         <v>Effect of changes in climate and land use on rice productivity in Adani, Nigeria</v>
       </c>
       <c r="E112" t="str">
-        <v>Arabian Journal of Geosciences</v>
-      </c>
-      <c r="F112" t="str">
-        <v/>
-      </c>
-      <c r="G112" t="str">
-        <v xml:space="preserve">Mama Cordelia Nnennaya; Nwonu Donald Chimobi; Odo Emmanuel Chukwuebuka; Ndichie Chinemelu Cosmas; Onyia Michael Ebie; </v>
-      </c>
-      <c r="H112" t="str">
         <v>2021</v>
-      </c>
-      <c r="I112" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="113">
@@ -3664,19 +2320,7 @@
         <v>Farmers’ adaptation to climate change and water consumption in southwest Iran: application of switching regression</v>
       </c>
       <c r="E113" t="str">
-        <v>Climate Research</v>
-      </c>
-      <c r="F113" t="str">
-        <v/>
-      </c>
-      <c r="G113" t="str">
-        <v xml:space="preserve">Mardani Najafabadi; M; Forouzani M; Nikmehr S; </v>
-      </c>
-      <c r="H113" t="str">
         <v>2024</v>
-      </c>
-      <c r="I113" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="114">
@@ -3693,19 +2337,7 @@
         <v>Dry spells assessment with reference to the maize crop in the Luvuvhu River catchment of South Africa</v>
       </c>
       <c r="E114" t="str">
-        <v>Physics and Chemistry of the Earth</v>
-      </c>
-      <c r="F114" t="str">
-        <v/>
-      </c>
-      <c r="G114" t="str">
-        <v xml:space="preserve">Masupha Teboho Elisa; Moeletsi Mokhele Edmond; Tsubo Mitsuru; </v>
-      </c>
-      <c r="H114" t="str">
         <v>2016</v>
-      </c>
-      <c r="I114" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="115">
@@ -3722,19 +2354,7 @@
         <v>Impact of COVID-19 among small-scale industry fishermen - A mixed methods study from the coastal area of Karnataka</v>
       </c>
       <c r="E115" t="str">
-        <v>Work</v>
-      </c>
-      <c r="F115" t="str">
-        <v/>
-      </c>
-      <c r="G115" t="str">
-        <v xml:space="preserve">Mathew Geethu; Srinivasan Manikandan; Kolangaredath Akshaya; Melur Sukumar; Gautam; Beerapa Ravichandran; Kumar Nanjesh; Nanjunda Sastry Thara; Kanchipamu Mohan Rao; </v>
-      </c>
-      <c r="H115" t="str">
         <v>2024</v>
-      </c>
-      <c r="I115" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="116">
@@ -3751,19 +2371,7 @@
         <v>Grazing intensity effects on rangeland condition and tree diversity in Afar, northeastern Ethiopia</v>
       </c>
       <c r="E116" t="str">
-        <v>Heliyon</v>
-      </c>
-      <c r="F116" t="str">
-        <v/>
-      </c>
-      <c r="G116" t="str">
-        <v xml:space="preserve">Mathewos Mengeste; Sisay Amsalu; Berhanu Yonas; </v>
-      </c>
-      <c r="H116" t="str">
         <v>2023</v>
-      </c>
-      <c r="I116" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="117">
@@ -3780,19 +2388,7 @@
         <v>Building resilience in Sub-Saharan Africa's food systems: Diversification, traceability, capacity building and technology for overcoming challenges</v>
       </c>
       <c r="E117" t="str">
-        <v>Food and Energy Security</v>
-      </c>
-      <c r="F117" t="str">
-        <v/>
-      </c>
-      <c r="G117" t="str">
-        <v xml:space="preserve">Mekonnen Solomon Abate; Jalata Dassalegn Daraje; Onyeaka Helen; </v>
-      </c>
-      <c r="H117" t="str">
         <v>2024</v>
-      </c>
-      <c r="I117" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="118">
@@ -3809,19 +2405,7 @@
         <v>A fresh look at shifting cultivation: Fallow length an uncertain indicator of productivity</v>
       </c>
       <c r="E118" t="str">
-        <v>Agricultural Systems</v>
-      </c>
-      <c r="F118" t="str">
-        <v/>
-      </c>
-      <c r="G118" t="str">
-        <v xml:space="preserve">Mertz Ole; Wadley Reed L; Nielsen Uffe; Bruun Thilde B; Colfer Carol J.P; de Neergaard Andreas; Jepsen Martin R; Martinussen Torben; Zhao Qiang; Noweg Gabriel T; Magid Jakob; </v>
-      </c>
-      <c r="H118" t="str">
         <v>2008</v>
-      </c>
-      <c r="I118" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="119">
@@ -3838,19 +2422,7 @@
         <v>Agro-Economic Evaluation of Alternative Crop Management Options for Teff Production in the Northwestern Highlands of Ethiopia</v>
       </c>
       <c r="E119" t="str">
-        <v>Agriculture Switzerland</v>
-      </c>
-      <c r="F119" t="str">
-        <v/>
-      </c>
-      <c r="G119" t="str">
-        <v xml:space="preserve">Mihretie Fekremariam Asargew; Tsunekawa Atsushi; Haregeweyn Nigussie; Adgo Enyew; Tsubo Mitsuru; Masunaga Tsugiyuki; Meshesha Derege Tsegaye; Ebabu Kindiye; Bayable Muluken; </v>
-      </c>
-      <c r="H119" t="str">
         <v>2021</v>
-      </c>
-      <c r="I119" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="120">
@@ -3867,19 +2439,7 @@
         <v>An approach for forecasting of public water scarcity at the end of the 21st century, in the Timiş Plain of Romania</v>
       </c>
       <c r="E120" t="str">
-        <v>Technological Forecasting and Social Change</v>
-      </c>
-      <c r="F120" t="str">
-        <v/>
-      </c>
-      <c r="G120" t="str">
-        <v xml:space="preserve">Mitrică Bianca; Mitrică Eugen; Enciu Petru; Mocanu Irena; </v>
-      </c>
-      <c r="H120" t="str">
         <v>2017</v>
-      </c>
-      <c r="I120" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="121">
@@ -3896,19 +2456,7 @@
         <v>Farm income, gender differentials and climate risk in Cameroon: Typology of male and female adaptation options across agroecologies</v>
       </c>
       <c r="E121" t="str">
-        <v>Sustainability Science</v>
-      </c>
-      <c r="F121" t="str">
-        <v/>
-      </c>
-      <c r="G121" t="str">
-        <v xml:space="preserve">Molua Ernest L; </v>
-      </c>
-      <c r="H121" t="str">
         <v>2011</v>
-      </c>
-      <c r="I121" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="122">
@@ -3925,19 +2473,7 @@
         <v>Agriculture on the brink: Climate change, labor and smallholder farming in Botswana</v>
       </c>
       <c r="E122" t="str">
-        <v>Land</v>
-      </c>
-      <c r="F122" t="str">
-        <v/>
-      </c>
-      <c r="G122" t="str">
-        <v xml:space="preserve">Moseley William; </v>
-      </c>
-      <c r="H122" t="str">
         <v>2016</v>
-      </c>
-      <c r="I122" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="123">
@@ -3954,19 +2490,7 @@
         <v>Implementation or inaction: how governmental multi-interventions catalyze farmers' adoption for climate adaption technology?</v>
       </c>
       <c r="E123" t="str">
-        <v>Journal of Cleaner Production</v>
-      </c>
-      <c r="F123" t="str">
-        <v/>
-      </c>
-      <c r="G123" t="str">
-        <v xml:space="preserve">Mu Lan; Li Ying; Liu Haoying; Wang Qiongyao; </v>
-      </c>
-      <c r="H123" t="str">
         <v>2025</v>
-      </c>
-      <c r="I123" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="124">
@@ -3983,19 +2507,7 @@
         <v>Adoption determinants of multiple climate smart agricultural technologies in Zimbabwe: Considerations for scaling-up and out</v>
       </c>
       <c r="E124" t="str">
-        <v>African Journal of Science Technology Innovation and Development</v>
-      </c>
-      <c r="F124" t="str">
-        <v/>
-      </c>
-      <c r="G124" t="str">
-        <v xml:space="preserve">Mujeyi Angeline; Mudhara Maxwell; Mutenje Munyaradzi J; </v>
-      </c>
-      <c r="H124" t="str">
         <v>2020</v>
-      </c>
-      <c r="I124" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="125">
@@ -4012,19 +2524,7 @@
         <v>The role of large traders in driving sustainable agricultural intensification in smallholder farms: Evidence from Kenya</v>
       </c>
       <c r="E125" t="str">
-        <v>Agricultural Economics United Kingdom</v>
-      </c>
-      <c r="F125" t="str">
-        <v/>
-      </c>
-      <c r="G125" t="str">
-        <v xml:space="preserve">Mulwa Chalmers K; Muyanga Milu; Visser Martine; </v>
-      </c>
-      <c r="H125" t="str">
         <v>2021</v>
-      </c>
-      <c r="I125" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="126">
@@ -4041,19 +2541,7 @@
         <v>Occupational Stress and Associated Factors among Sugarcane Farmers in Sa Kaeo Province, Thailand</v>
       </c>
       <c r="E126" t="str">
-        <v>Journal of Current Science and Technology</v>
-      </c>
-      <c r="F126" t="str">
-        <v/>
-      </c>
-      <c r="G126" t="str">
-        <v xml:space="preserve">Mungkhunthod Sootthikarn; Tanthanapanyakorn Phannathat; Khantikulanon Nonlapan; Praserttai Chaninan; </v>
-      </c>
-      <c r="H126" t="str">
         <v>2026</v>
-      </c>
-      <c r="I126" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="127">
@@ -4070,19 +2558,7 @@
         <v>Climate change-induced drought impacts, adaptation and mitigation measures in semi-arid pastoral and agricultural watersheds</v>
       </c>
       <c r="E127" t="str">
-        <v>Sustainability Switzerland</v>
-      </c>
-      <c r="F127" t="str">
-        <v/>
-      </c>
-      <c r="G127" t="str">
-        <v xml:space="preserve">Muralikrishnan Lakshmanan; Padaria Rabindra N; Choudhary Anil K; Dass Anchal; Shokralla Shadi; El-Abedin Tarek K. Zin; Abdelmohsen Shadi A. M; Mahmoud Eman A; Elansary Hosam O; </v>
-      </c>
-      <c r="H127" t="str">
         <v>2022</v>
-      </c>
-      <c r="I127" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="128">
@@ -4099,19 +2575,7 @@
         <v>Understanding Farmer Typology, Manure Use Dynamics and Resource Endowment in a Smallholder Rural Community of the Eastern Cape Province, South Africa</v>
       </c>
       <c r="E128" t="str">
-        <v>South African Journal of Agricultural Extension</v>
-      </c>
-      <c r="F128" t="str">
-        <v/>
-      </c>
-      <c r="G128" t="str">
-        <v xml:space="preserve">Mzayiya Z B; Manyevere A; Mashamaite C V; </v>
-      </c>
-      <c r="H128" t="str">
         <v>2025</v>
-      </c>
-      <c r="I128" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="129">
@@ -4128,19 +2592,7 @@
         <v>Meteorological information utilization and adoption of climate-smart agricultural practices; modifying factors and mediating effect</v>
       </c>
       <c r="E129" t="str">
-        <v>Environmental Development</v>
-      </c>
-      <c r="F129" t="str">
-        <v/>
-      </c>
-      <c r="G129" t="str">
-        <v xml:space="preserve">Nantongo Beckie; Ssekandi Joseph; Ngom Ablaye; Dieng Birane; Diouf Ndongo; Diouf Jules; Noba Kandioura; </v>
-      </c>
-      <c r="H129" t="str">
         <v>2023</v>
-      </c>
-      <c r="I129" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="130">
@@ -4157,19 +2609,7 @@
         <v>The evolution of farm animal biotechnology</v>
       </c>
       <c r="E130" t="str">
-        <v>Animal Biotechnology 1 Reproductive Biotechnologies</v>
-      </c>
-      <c r="F130" t="str">
-        <v/>
-      </c>
-      <c r="G130" t="str">
-        <v xml:space="preserve">Niemann Heiner; Seamark Bob; </v>
-      </c>
-      <c r="H130" t="str">
         <v>2018</v>
-      </c>
-      <c r="I130" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="131">
@@ -4186,19 +2626,7 @@
         <v>Droughts, biodiversity, and rural incomes in the tropics</v>
       </c>
       <c r="E131" t="str">
-        <v>Journal of the Association of Environmental and Resource Economists</v>
-      </c>
-      <c r="F131" t="str">
-        <v/>
-      </c>
-      <c r="G131" t="str">
-        <v xml:space="preserve">Noack Frederik; Riekhof Marie-Catherine; Di Falco Salvatore; </v>
-      </c>
-      <c r="H131" t="str">
         <v>2019</v>
-      </c>
-      <c r="I131" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="132">
@@ -4215,19 +2643,7 @@
         <v>Farmers’ knowledge, attitude, and motivation for adoption of climate-smart agroforestry in two contrasting agroecosystems of Rwanda</v>
       </c>
       <c r="E132" t="str">
-        <v>Trees Forests and People</v>
-      </c>
-      <c r="F132" t="str">
-        <v/>
-      </c>
-      <c r="G132" t="str">
-        <v xml:space="preserve">Ntawuruhunga Donatien; Ngowi Edwin Estomii; Mangi Halima Omari; Salanga Raymond John; Leonard Kenneth Lynch; </v>
-      </c>
-      <c r="H132" t="str">
         <v>2025</v>
-      </c>
-      <c r="I132" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="133">
@@ -4244,19 +2660,7 @@
         <v>Optimization of rainwater harvesting system design for smallholder irrigation farmers in Kenya: A review</v>
       </c>
       <c r="E133" t="str">
-        <v>Aqua Water Infrastructure Ecosystems and Society</v>
-      </c>
-      <c r="F133" t="str">
-        <v/>
-      </c>
-      <c r="G133" t="str">
-        <v xml:space="preserve">Odhiambo Kevin O; Iro Ong'or; Basil T; Kanda Edwin K; </v>
-      </c>
-      <c r="H133" t="str">
         <v>2021</v>
-      </c>
-      <c r="I133" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="134">
@@ -4273,19 +2677,7 @@
         <v>Climate Change Impacts on Environment: Human Displacement and Social Conflicts in Nigeria</v>
       </c>
       <c r="E134" t="str">
-        <v>Iop Conference Series Earth and Environmental Science</v>
-      </c>
-      <c r="F134" t="str">
-        <v/>
-      </c>
-      <c r="G134" t="str">
-        <v xml:space="preserve">Olagunju T E; Adewoye S O; Adewoye A O; Opasola O A; </v>
-      </c>
-      <c r="H134" t="str">
         <v>2021</v>
-      </c>
-      <c r="I134" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="135">
@@ -4302,19 +2694,7 @@
         <v>Intensity of adaptations to heat stress in poultry farms: A behavioural analysis of farmers in Ondo state, Nigeria</v>
       </c>
       <c r="E135" t="str">
-        <v>Journal of Thermal Biology</v>
-      </c>
-      <c r="F135" t="str">
-        <v/>
-      </c>
-      <c r="G135" t="str">
-        <v xml:space="preserve">Olutumise Adewale Isaac; </v>
-      </c>
-      <c r="H135" t="str">
         <v>2023</v>
-      </c>
-      <c r="I135" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="136">
@@ -4331,19 +2711,7 @@
         <v>Forest Resource Use and Management in Nigeria: Implications for Implementation of REDD+ for Climate Change Mitigation in West Africa</v>
       </c>
       <c r="E136" t="str">
-        <v>Handbook of Climate Change Management Research Leadership Transformation</v>
-      </c>
-      <c r="F136" t="str">
-        <v/>
-      </c>
-      <c r="G136" t="str">
-        <v xml:space="preserve">Onyekuru NwaJesus Anthony; Marchant Rob; Ihemezie Eberechukwu Johnpaul; </v>
-      </c>
-      <c r="H136" t="str">
         <v>2021</v>
-      </c>
-      <c r="I136" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="137">
@@ -4360,19 +2728,7 @@
         <v>Climate change perception and uptake of climate-smart agriculture in rice production in ebonyi state, nigeria</v>
       </c>
       <c r="E137" t="str">
-        <v>Atmosphere</v>
-      </c>
-      <c r="F137" t="str">
-        <v/>
-      </c>
-      <c r="G137" t="str">
-        <v xml:space="preserve">Onyeneke Robert Ugochukwu; Amadi Mark Umunna; Njoku Chukwudi Loveday; Osuji Emeka Emmanuel; </v>
-      </c>
-      <c r="H137" t="str">
         <v>2021</v>
-      </c>
-      <c r="I137" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="138">
@@ -4389,19 +2745,7 @@
         <v>Diversifying to alleviate poverty? A bibliometric analysis of the relationship between agricultural strategies and multidimensional poverty in rural Côte d’Ivoire</v>
       </c>
       <c r="E138" t="str">
-        <v>Cogent Economics and Finance</v>
-      </c>
-      <c r="F138" t="str">
-        <v/>
-      </c>
-      <c r="G138" t="str">
-        <v xml:space="preserve">Ouedraogo Abdoul Rahmane; Kone Sita; Zoungrana Tibi Didier; </v>
-      </c>
-      <c r="H138" t="str">
         <v>2025</v>
-      </c>
-      <c r="I138" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="139">
@@ -4418,19 +2762,7 @@
         <v>Emerging threats to food security in Nigeria: Way forward</v>
       </c>
       <c r="E139" t="str">
-        <v>Emerging Challenges to Food Production and Security in Asia Middle East and Africa Climate Risks and Resource Scarcity</v>
-      </c>
-      <c r="F139" t="str">
-        <v/>
-      </c>
-      <c r="G139" t="str">
-        <v xml:space="preserve">Ozkan Burhan; Fawole Wasiu Olayinka; </v>
-      </c>
-      <c r="H139" t="str">
         <v>2021</v>
-      </c>
-      <c r="I139" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="140">
@@ -4447,19 +2779,7 @@
         <v>Gender transformative impacts from watershed interventions: Insights from a mixed-methods study in the Bundelkhand region of India</v>
       </c>
       <c r="E140" t="str">
-        <v>Transactions of the Asabe</v>
-      </c>
-      <c r="F140" t="str">
-        <v/>
-      </c>
-      <c r="G140" t="str">
-        <v xml:space="preserve">Padmaja R; Kavitha K; Pramanik S; Duche V D; Singh Y U; Whitbread A M; Singh R; Garg K K; Leder S; </v>
-      </c>
-      <c r="H140" t="str">
         <v>2020</v>
-      </c>
-      <c r="I140" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="141">
@@ -4476,19 +2796,7 @@
         <v>Adoption of climate-smart agriculture technology in drought-prone area of India – implications on farmers' livelihoods</v>
       </c>
       <c r="E141" t="str">
-        <v>Journal of Agribusiness in Developing and Emerging Economies</v>
-      </c>
-      <c r="F141" t="str">
-        <v/>
-      </c>
-      <c r="G141" t="str">
-        <v xml:space="preserve">Pal Barun Deb; Kapoor Shreya; Saroj Sunil; Jat M L; Kumar Yogesh; Anantha K H; </v>
-      </c>
-      <c r="H141" t="str">
         <v>2022</v>
-      </c>
-      <c r="I141" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="142">
@@ -4505,19 +2813,7 @@
         <v>Community-based approaches to support the anchoring of climate-smart agriculture in Tanzania</v>
       </c>
       <c r="E142" t="str">
-        <v>Frontiers in Climate</v>
-      </c>
-      <c r="F142" t="str">
-        <v/>
-      </c>
-      <c r="G142" t="str">
-        <v xml:space="preserve">Pamuk Haki; van Asseldonk Marcel; Wattel Cor; Ng'ang'a Stanley Karanja; Hella Joseph Philip; Ruben Ruerd; </v>
-      </c>
-      <c r="H142" t="str">
         <v>2022</v>
-      </c>
-      <c r="I142" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="143">
@@ -4534,19 +2830,7 @@
         <v>Participatory Evaluation and Pre-Extension Demonstration of Improved Finger Millet Varieties with Its Full Package in Selected Districts of Debub Omo Zone, Southern Ethiopia</v>
       </c>
       <c r="E143" t="str">
-        <v>International Journal of Agricultural Science Research and Technology in Extension and Education Systems</v>
-      </c>
-      <c r="F143" t="str">
-        <v/>
-      </c>
-      <c r="G143" t="str">
-        <v/>
-      </c>
-      <c r="H143" t="str">
         <v>2021</v>
-      </c>
-      <c r="I143" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="144">
@@ -4563,19 +2847,7 @@
         <v>Mitigating greenhouse gas and nitrogen loss with improved fertilizer management in rice: Quantification and economic assessment</v>
       </c>
       <c r="E144" t="str">
-        <v>Nutrient Cycling in Agroecosystems</v>
-      </c>
-      <c r="F144" t="str">
-        <v/>
-      </c>
-      <c r="G144" t="str">
-        <v xml:space="preserve">Pathak H; </v>
-      </c>
-      <c r="H144" t="str">
         <v>2010</v>
-      </c>
-      <c r="I144" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="145">
@@ -4592,19 +2864,7 @@
         <v>Assessing multi-scale vulnerability of fisheries of Vembanad lake, Peninsular India, due to climate change: a stakeholders-based approach</v>
       </c>
       <c r="E145" t="str">
-        <v>Environment Development and Sustainability</v>
-      </c>
-      <c r="F145" t="str">
-        <v/>
-      </c>
-      <c r="G145" t="str">
-        <v xml:space="preserve">Paul Thankam Theresa; Sarkar U K; Salim Shyam S; Manoharan S; Ganeshan Kuberan; Das B K; </v>
-      </c>
-      <c r="H145" t="str">
         <v>2024</v>
-      </c>
-      <c r="I145" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="146">
@@ -4621,19 +2881,7 @@
         <v>Fishers' ecological knowledge points to fishing-induced changes in the Peruvian Amazon</v>
       </c>
       <c r="E146" t="str">
-        <v>Ecological Applications</v>
-      </c>
-      <c r="F146" t="str">
-        <v/>
-      </c>
-      <c r="G146" t="str">
-        <v xml:space="preserve">Poissant David; Coomes Oliver T; Robinson Brian E; Vargas Dávila; Gladys; </v>
-      </c>
-      <c r="H146" t="str">
         <v>2024</v>
-      </c>
-      <c r="I146" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="147">
@@ -4650,19 +2898,7 @@
         <v>Sowing the wheat seeds of Afghanistan's future</v>
       </c>
       <c r="E147" t="str">
-        <v>Plants People Planet</v>
-      </c>
-      <c r="F147" t="str">
-        <v/>
-      </c>
-      <c r="G147" t="str">
-        <v xml:space="preserve">Poole Nigel; Sharma Rajiv; Nemat Orzala A; Trenchard Richard; Scanlon Andrew; Davy Charles; Ataei Najibeh; Donovan Jason; Bentley Alison R; </v>
-      </c>
-      <c r="H147" t="str">
         <v>2022</v>
-      </c>
-      <c r="I147" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="148">
@@ -4679,19 +2915,7 @@
         <v>Production of Browse Trees/Shrubs under Climate Change Conditions in the Butana Rangelands of Sudan</v>
       </c>
       <c r="E148" t="str">
-        <v>Journal of Rangeland Science</v>
-      </c>
-      <c r="F148" t="str">
-        <v/>
-      </c>
-      <c r="G148" t="str">
-        <v/>
-      </c>
-      <c r="H148" t="str">
         <v>2024</v>
-      </c>
-      <c r="I148" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="149">
@@ -4708,19 +2932,7 @@
         <v>Productive, economic and greenhouse gases modelling of typical beef cow-calf systems in the flooding Pampas.</v>
       </c>
       <c r="E149" t="str">
-        <v>Chilean Journal of Agricultural and Animal Sciences</v>
-      </c>
-      <c r="F149" t="str">
-        <v/>
-      </c>
-      <c r="G149" t="str">
-        <v/>
-      </c>
-      <c r="H149" t="str">
         <v>2019</v>
-      </c>
-      <c r="I149" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="150">
@@ -4737,19 +2949,7 @@
         <v>Responses of fish production to fishing and climate variability in the northern South China Sea</v>
       </c>
       <c r="E150" t="str">
-        <v>Progress in Oceanography</v>
-      </c>
-      <c r="F150" t="str">
-        <v/>
-      </c>
-      <c r="G150" t="str">
-        <v xml:space="preserve">Qiu Yongsong; Lin Zhaojin; Wang Yuezhong; </v>
-      </c>
-      <c r="H150" t="str">
         <v>2010</v>
-      </c>
-      <c r="I150" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="151">
@@ -4766,19 +2966,7 @@
         <v>Targeting management practices for rice yield gains in stress-prone environments of Myanmar</v>
       </c>
       <c r="E151" t="str">
-        <v>Field Crops Research</v>
-      </c>
-      <c r="F151" t="str">
-        <v/>
-      </c>
-      <c r="G151" t="str">
-        <v xml:space="preserve">Radanielson A M; Kato Yoichiro; Palao Leo Kris; Feyisa Gudina; Malabayabas Arelene Julia; Aunario Jorrel K; Garcia Cornelia; Balanza Jane G; Win Khin Thawda; Singh Rakesh K; Zamora Chenie; Myint Daw Tin Tin; Johnson David E; </v>
-      </c>
-      <c r="H151" t="str">
         <v>2019</v>
-      </c>
-      <c r="I151" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="152">
@@ -4795,19 +2983,7 @@
         <v>Present status and approaches for the sustainable development of community based fish culture in seasonal floodplains of Bangladesh</v>
       </c>
       <c r="E152" t="str">
-        <v>Pakistan Journal of Biological Sciences</v>
-      </c>
-      <c r="F152" t="str">
-        <v/>
-      </c>
-      <c r="G152" t="str">
-        <v xml:space="preserve">Rahman M F; Jalal K C.A; Jahan Nasrin; Kamaruzzam B Y; Ara R; Arshad A; </v>
-      </c>
-      <c r="H152" t="str">
         <v>2012</v>
-      </c>
-      <c r="I152" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="153">
@@ -4824,19 +3000,7 @@
         <v>Climate Change Related Factors Impacting Dairy Production in Pakistan</v>
       </c>
       <c r="E153" t="str">
-        <v>Pakistan Journal of Agricultural Research</v>
-      </c>
-      <c r="F153" t="str">
-        <v/>
-      </c>
-      <c r="G153" t="str">
-        <v xml:space="preserve">Rahman Muhammad Abdul; Saboor Abdul; Hameed Gulnaz; Bilal Ghulam; Tanwir Farooq; </v>
-      </c>
-      <c r="H153" t="str">
         <v>2019</v>
-      </c>
-      <c r="I153" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="154">
@@ -4853,19 +3017,7 @@
         <v>Livelihoods and vulnerabilities of small-scale fishers to the impacts of climate variability and change: Insights from the coastal areas of bangladesh</v>
       </c>
       <c r="E154" t="str">
-        <v>Egyptian Journal of Aquatic Biology and Fisheries</v>
-      </c>
-      <c r="F154" t="str">
-        <v/>
-      </c>
-      <c r="G154" t="str">
-        <v xml:space="preserve">Rahman Sunny et al; Atiqur; </v>
-      </c>
-      <c r="H154" t="str">
         <v>2021</v>
-      </c>
-      <c r="I154" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="155">
@@ -4882,19 +3034,7 @@
         <v>Predicting intention in applying solar energy technologies in agriculture industry: A moderated and mediated model</v>
       </c>
       <c r="E155" t="str">
-        <v>Cleaner and Responsible Consumption</v>
-      </c>
-      <c r="F155" t="str">
-        <v/>
-      </c>
-      <c r="G155" t="str">
-        <v xml:space="preserve">Rahmani Amir; Bonyadi Naeini Ali; </v>
-      </c>
-      <c r="H155" t="str">
         <v>2023</v>
-      </c>
-      <c r="I155" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="156">
@@ -4911,19 +3051,7 @@
         <v>Climate Shocks and Social Networks: Understanding Adaptation among Rural Indian Households</v>
       </c>
       <c r="E156" t="str">
-        <v>Climate</v>
-      </c>
-      <c r="F156" t="str">
-        <v/>
-      </c>
-      <c r="G156" t="str">
-        <v xml:space="preserve">Ramsawak Richard Anthony; </v>
-      </c>
-      <c r="H156" t="str">
         <v>2022</v>
-      </c>
-      <c r="I156" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="157">
@@ -4940,19 +3068,7 @@
         <v>Flood risk mapping of the flood-prone Rangpur division of Bangladesh using remote sensing and multi-criteria analysis</v>
       </c>
       <c r="E157" t="str">
-        <v>Natural Hazards Research</v>
-      </c>
-      <c r="F157" t="str">
-        <v/>
-      </c>
-      <c r="G157" t="str">
-        <v xml:space="preserve">Rana S M. Sohel; Habib SM Ahsan; Sharifee M Nur Hossain; Sultana Nasrin; Rahman Syed Hafizur; </v>
-      </c>
-      <c r="H157" t="str">
         <v>2024</v>
-      </c>
-      <c r="I157" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="158">
@@ -4969,19 +3085,7 @@
         <v>Resilience of coastal agricultural systems in Bangladesh: Assessment for agroecosystem stewardship strategies</v>
       </c>
       <c r="E158" t="str">
-        <v>Ecological Indicators</v>
-      </c>
-      <c r="F158" t="str">
-        <v/>
-      </c>
-      <c r="G158" t="str">
-        <v xml:space="preserve">Roy Ranjan; Gain Animesh K; Samat Narimah; Hurlbert Margot; Tan Mou Leong; Chan Ngai Weng; </v>
-      </c>
-      <c r="H158" t="str">
         <v>2019</v>
-      </c>
-      <c r="I158" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="159">
@@ -4998,19 +3102,7 @@
         <v>Unwrapping the memory box: Gendered livelihoods in a forest community in the Sundarbans, Bangladesh</v>
       </c>
       <c r="E159" t="str">
-        <v>Asian Journal of Social Science</v>
-      </c>
-      <c r="F159" t="str">
-        <v/>
-      </c>
-      <c r="G159" t="str">
-        <v xml:space="preserve">Roy Sajal; Zafarullah Habib; Das Arunima Kishore; </v>
-      </c>
-      <c r="H159" t="str">
         <v>2020</v>
-      </c>
-      <c r="I159" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="160">
@@ -5027,19 +3119,7 @@
         <v>Interconnections between health, environment, demographic, and livelihood factors: shaping food security in Rukiga, Uganda</v>
       </c>
       <c r="E160" t="str">
-        <v>Elgar Companion to Health and the Sustainable Development Goals</v>
-      </c>
-      <c r="F160" t="str">
-        <v/>
-      </c>
-      <c r="G160" t="str">
-        <v xml:space="preserve">Ruhi Tashfiha Nusrat; Muhumuza Richard; Namanya Gift; Mayhew Susannah H; </v>
-      </c>
-      <c r="H160" t="str">
         <v>2025</v>
-      </c>
-      <c r="I160" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="161">
@@ -5056,19 +3136,7 @@
         <v>Flood Mapping and Damage Analysis Using Multispectral Sentinel-2 Satellite Imagery and Machine Learning Techniques</v>
       </c>
       <c r="E161" t="str">
-        <v>Recent Advances in Computer Science and Communications</v>
-      </c>
-      <c r="F161" t="str">
-        <v/>
-      </c>
-      <c r="G161" t="str">
-        <v xml:space="preserve">Saini Rashmi; Rawat Shivam; Singh Suraj; Semwal Prabhakar; </v>
-      </c>
-      <c r="H161" t="str">
         <v>2025</v>
-      </c>
-      <c r="I161" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="162">
@@ -5085,19 +3153,7 @@
         <v>Impact of Viral Diseases on the Livestock Sector in Bangladesh</v>
       </c>
       <c r="E162" t="str">
-        <v>Veterinary Medicine International</v>
-      </c>
-      <c r="F162" t="str">
-        <v/>
-      </c>
-      <c r="G162" t="str">
-        <v xml:space="preserve">Salauddin Md; Khan Md Ahanaf Ajmaeen; Rahmati Azri; Hossain Md Golzar; Shimada Masaru; Saha Sukumar; </v>
-      </c>
-      <c r="H162" t="str">
         <v>2025</v>
-      </c>
-      <c r="I162" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="163">
@@ -5114,19 +3170,7 @@
         <v>A theoretical assessment of the environmental change from floodplain rice fields to irrigated perimeters: A case study in the San Francisco Sergipano Low Valley in the Northeast Region of Brazil</v>
       </c>
       <c r="E163" t="str">
-        <v>Wit Transactions on Ecology and the Environment</v>
-      </c>
-      <c r="F163" t="str">
-        <v/>
-      </c>
-      <c r="G163" t="str">
-        <v xml:space="preserve">SANTOS GEDÁLIA C; </v>
-      </c>
-      <c r="H163" t="str">
         <v>2017</v>
-      </c>
-      <c r="I163" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="164">
@@ -5143,19 +3187,7 @@
         <v>Climate-induced coastal occupational vulnerability and livelihood insecurity: Insights from coastal Bangladesh</v>
       </c>
       <c r="E164" t="str">
-        <v>Progress in Disaster Science</v>
-      </c>
-      <c r="F164" t="str">
-        <v/>
-      </c>
-      <c r="G164" t="str">
-        <v xml:space="preserve">Sarkar Monishankar; Paul Subrata; Garai Joydeb; </v>
-      </c>
-      <c r="H164" t="str">
         <v>2024</v>
-      </c>
-      <c r="I164" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="165">
@@ -5172,19 +3204,7 @@
         <v>The combination of climate information services in the decision-making process of farmers to reduce climate risks: Application of social cognition theory</v>
       </c>
       <c r="E165" t="str">
-        <v>Climate Services</v>
-      </c>
-      <c r="F165" t="str">
-        <v/>
-      </c>
-      <c r="G165" t="str">
-        <v xml:space="preserve">Savari Moslem; Zhoolideh Milad; Limuie Mohammad; </v>
-      </c>
-      <c r="H165" t="str">
         <v>2024</v>
-      </c>
-      <c r="I165" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="166">
@@ -5201,19 +3221,7 @@
         <v>Deep Learning Models and Their Ensembles for Robust Agricultural Yield Prediction in Saudi Arabia</v>
       </c>
       <c r="E166" t="str">
-        <v>Sustainability Switzerland</v>
-      </c>
-      <c r="F166" t="str">
-        <v/>
-      </c>
-      <c r="G166" t="str">
-        <v xml:space="preserve">Sbai Zohra; </v>
-      </c>
-      <c r="H166" t="str">
         <v>2025</v>
-      </c>
-      <c r="I166" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="167">
@@ -5230,19 +3238,7 @@
         <v>Scaling up agroforestry to achieve food security and environmental protection among smallholder farmers in Malawi</v>
       </c>
       <c r="E167" t="str">
-        <v>Field Actions Science Report</v>
-      </c>
-      <c r="F167" t="str">
-        <v/>
-      </c>
-      <c r="G167" t="str">
-        <v/>
-      </c>
-      <c r="H167" t="str">
         <v>2012</v>
-      </c>
-      <c r="I167" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="168">
@@ -5259,19 +3255,7 @@
         <v>Applied nucleation under high biodiversity silvopastoral system as an adaptive strategy against microclimate extremes in pasture areas</v>
       </c>
       <c r="E168" t="str">
-        <v>International Journal of Biometeorology</v>
-      </c>
-      <c r="F168" t="str">
-        <v/>
-      </c>
-      <c r="G168" t="str">
-        <v xml:space="preserve">Schmitt Filho; Abdon L; Kretzer Stéfano Gomes; Farley Joshua; Kazama Daniele C; Sinisgalli Paulo A; Deniz Matheus; </v>
-      </c>
-      <c r="H168" t="str">
         <v>2023</v>
-      </c>
-      <c r="I168" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="169">
@@ -5288,19 +3272,7 @@
         <v>Satellite-based multi-annual yield models for major food crops at the household field level for nutrition and health research: A case study from the Nouna HDSS, Burkina Faso</v>
       </c>
       <c r="E169" t="str">
-        <v>International Journal of Applied Earth Observation and Geoinformation</v>
-      </c>
-      <c r="F169" t="str">
-        <v/>
-      </c>
-      <c r="G169" t="str">
-        <v xml:space="preserve">Schwarz Maximilian; Ouédraogo Windpanga Aristide; Traoré Issouf; Müller Charlotte; Sié Ali; Barteit Sandra; Mank Isabel; Siegert Florian; Sauerborn Rainer; Franke Jonas; </v>
-      </c>
-      <c r="H169" t="str">
         <v>2023</v>
-      </c>
-      <c r="I169" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="170">
@@ -5317,19 +3289,7 @@
         <v>The challenge of making climate adaptation profitable for farmers: evidence from Sri Lanka's rice sector</v>
       </c>
       <c r="E170" t="str">
-        <v>Environment and Development Economics</v>
-      </c>
-      <c r="F170" t="str">
-        <v/>
-      </c>
-      <c r="G170" t="str">
-        <v xml:space="preserve">Scognamillo Antonio; Sitko Nicholas; Bandara Sidath; Hewage Shantha; Munaweera Thilani; Kwon Jihae; </v>
-      </c>
-      <c r="H170" t="str">
         <v>2022</v>
-      </c>
-      <c r="I170" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="171">
@@ -5346,19 +3306,7 @@
         <v>Key factors affecting the flood vulnerability and adaptation of the shrimp farming sector in Thailand</v>
       </c>
       <c r="E171" t="str">
-        <v>International Journal of Disaster Risk Reduction</v>
-      </c>
-      <c r="F171" t="str">
-        <v/>
-      </c>
-      <c r="G171" t="str">
-        <v xml:space="preserve">Seekao Chaiyaporn; Pharino Chanathip; </v>
-      </c>
-      <c r="H171" t="str">
         <v>2016</v>
-      </c>
-      <c r="I171" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="172">
@@ -5375,19 +3323,7 @@
         <v>Determination of seroprevalence of contagious caprine pleuropneumonia and associated risk factors in goats and sheep using classification and regression tree</v>
       </c>
       <c r="E172" t="str">
-        <v>Animals</v>
-      </c>
-      <c r="F172" t="str">
-        <v/>
-      </c>
-      <c r="G172" t="str">
-        <v xml:space="preserve">Selim Abdelfattah; Megahed Ameer; Kandeel Sahar; Alanazi Abdullah D; Almohammed Hamdan I; </v>
-      </c>
-      <c r="H172" t="str">
         <v>2021</v>
-      </c>
-      <c r="I172" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="173">
@@ -5404,19 +3340,7 @@
         <v>Determinants of reactive adaptations to climate change in semi-arid region of Pakistan</v>
       </c>
       <c r="E173" t="str">
-        <v>Journal of Arid Environments</v>
-      </c>
-      <c r="F173" t="str">
-        <v/>
-      </c>
-      <c r="G173" t="str">
-        <v xml:space="preserve">Shahid Rabia; Shijie Li; Shahid Sidra; Altaf Muhammad Ahsan; Shahid Humera; </v>
-      </c>
-      <c r="H173" t="str">
         <v>2021</v>
-      </c>
-      <c r="I173" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="174">
@@ -5433,19 +3357,7 @@
         <v>Effect of Climate Variability on Crop Income in Central Highlands of Ethiopia</v>
       </c>
       <c r="E174" t="str">
-        <v>Handbook of Climate Change Resilience Volume 1 4</v>
-      </c>
-      <c r="F174" t="str">
-        <v/>
-      </c>
-      <c r="G174" t="str">
-        <v xml:space="preserve">Shumetie Arega; Belay Kassa; Goshu Degye; Mwanjalolo Majaliwa; </v>
-      </c>
-      <c r="H174" t="str">
         <v>2019</v>
-      </c>
-      <c r="I174" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="175">
@@ -5462,19 +3374,7 @@
         <v>Adapting to climate change amidst innovation diffusion and declining indigenous agricultural knowledge and practices in Ghana</v>
       </c>
       <c r="E175" t="str">
-        <v>African Journal of Science Technology Innovation and Development</v>
-      </c>
-      <c r="F175" t="str">
-        <v/>
-      </c>
-      <c r="G175" t="str">
-        <v xml:space="preserve">Siakwah Pius; Ablo Austin Dziwornu; Sheburah-Essien Rosina; Zaami Mariama; Yaro Joseph Awetori; </v>
-      </c>
-      <c r="H175" t="str">
         <v>2025</v>
-      </c>
-      <c r="I175" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="176">
@@ -5491,19 +3391,7 @@
         <v>Identification of Minimum Data Set Under Balanced Fertilization for Sustainable Rice Production and Maintaining Soil Quality in Alluvial Soils of Eastern India</v>
       </c>
       <c r="E176" t="str">
-        <v>Communications in Soil Science and Plant Analysis</v>
-      </c>
-      <c r="F176" t="str">
-        <v/>
-      </c>
-      <c r="G176" t="str">
-        <v xml:space="preserve">Singh Shiv Ram; Kundu Dilip Kumar; Dey Pradip; Mahapatra Bikash Singha; </v>
-      </c>
-      <c r="H176" t="str">
         <v>2017</v>
-      </c>
-      <c r="I176" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="177">
@@ -5520,19 +3408,7 @@
         <v>The potential risks of climate change and weather index insurance scheme for Thailand's economic crop production</v>
       </c>
       <c r="E177" t="str">
-        <v>Environmental Challenges</v>
-      </c>
-      <c r="F177" t="str">
-        <v/>
-      </c>
-      <c r="G177" t="str">
-        <v xml:space="preserve">Sinnarong Nirote; Kuson Siwarat; Nunthasen Waraporn; Puphoung Sasiwimon; Souvannasouk Vannasinh; </v>
-      </c>
-      <c r="H177" t="str">
         <v>2022</v>
-      </c>
-      <c r="I177" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="178">
@@ -5549,19 +3425,7 @@
         <v>Impact of climatic variables on the spatial and temporal variability of crop yield and biomass gap in Sub-Saharan Africa- a case study in Central Ghana</v>
       </c>
       <c r="E178" t="str">
-        <v>Field Crops Research</v>
-      </c>
-      <c r="F178" t="str">
-        <v/>
-      </c>
-      <c r="G178" t="str">
-        <v xml:space="preserve">Srivastava Amit Kumar; Mboh Cho Miltin; Gaiser Thomas; Ewert Frank; </v>
-      </c>
-      <c r="H178" t="str">
         <v>2017</v>
-      </c>
-      <c r="I178" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="179">
@@ -5578,19 +3442,7 @@
         <v>ClimeGreAq: A software-based DSS for the climate change adaptation of Greek aquaculture</v>
       </c>
       <c r="E179" t="str">
-        <v>Environmental Modelling and Software</v>
-      </c>
-      <c r="F179" t="str">
-        <v/>
-      </c>
-      <c r="G179" t="str">
-        <v xml:space="preserve">Stavrakidis-Zachou Orestis; Sturm Astrid; Lika Konstadia; Wätzold Frank; Papandroulakis Nikos; </v>
-      </c>
-      <c r="H179" t="str">
         <v>2021</v>
-      </c>
-      <c r="I179" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="180">
@@ -5607,19 +3459,7 @@
         <v>Challenges and opportunities in building community-driven adaptive capacity under climate change for smallholder farmers in the Global South</v>
       </c>
       <c r="E180" t="str">
-        <v>International Journal of Climate Change Strategies and Management</v>
-      </c>
-      <c r="F180" t="str">
-        <v/>
-      </c>
-      <c r="G180" t="str">
-        <v xml:space="preserve">Stewart Iris T; Baez Morales; Allan; Maurer Edwin P; Li Qiuwen; Díaz Raúl Sandro; Guingona Briana; Torres Torres Landa; Arturo; </v>
-      </c>
-      <c r="H180" t="str">
         <v>2026</v>
-      </c>
-      <c r="I180" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="181">
@@ -5636,19 +3476,7 @@
         <v>Enhancing sugarcane growth quality and productivity through a biotechnology approach</v>
       </c>
       <c r="E181" t="str">
-        <v>Bio Web of Conferences</v>
-      </c>
-      <c r="F181" t="str">
-        <v/>
-      </c>
-      <c r="G181" t="str">
-        <v xml:space="preserve">Sugiharto Bambang; </v>
-      </c>
-      <c r="H181" t="str">
         <v>2024</v>
-      </c>
-      <c r="I181" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="182">
@@ -5665,19 +3493,7 @@
         <v>Analysis of human activities and socioeconomic development on the marine ecological carrying capacity (mecc) evaluation index to climate change adaptation in Nunukan Regency, North Kalimantan, Indonesia</v>
       </c>
       <c r="E182" t="str">
-        <v>Iop Conference Series Earth and Environmental Science</v>
-      </c>
-      <c r="F182" t="str">
-        <v/>
-      </c>
-      <c r="G182" t="str">
-        <v xml:space="preserve">Susandi A; Wijaya A; Kuntoro W S; Faisal I; Kertabudi F G; Nurdin I; </v>
-      </c>
-      <c r="H182" t="str">
         <v>2021</v>
-      </c>
-      <c r="I182" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="183">
@@ -5694,19 +3510,7 @@
         <v>Does adoption of multiple climate-smart practices improve farmers' climate resilience? Empirical evidence from the Nile Basin of Ethiopia</v>
       </c>
       <c r="E183" t="str">
-        <v>Climate Change Economics</v>
-      </c>
-      <c r="F183" t="str">
-        <v/>
-      </c>
-      <c r="G183" t="str">
-        <v xml:space="preserve">TEKLEWOLD HAILEMARIAM; MEKONNEN ALEMU; KOHLIN GUNNAR; DI FALCO SALVATORE; </v>
-      </c>
-      <c r="H183" t="str">
         <v>2017</v>
-      </c>
-      <c r="I183" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="184">
@@ -5723,19 +3527,7 @@
         <v>Modeling the impact of climate change on the environmental flow indicators over Omo-Gibe basin, Ethiopia</v>
       </c>
       <c r="E184" t="str">
-        <v>Modeling Earth Systems and Environment</v>
-      </c>
-      <c r="F184" t="str">
-        <v/>
-      </c>
-      <c r="G184" t="str">
-        <v xml:space="preserve">Tesfaye Tewodros Woldemariam; Dhanya C T; Gosain A K; </v>
-      </c>
-      <c r="H184" t="str">
         <v>2020</v>
-      </c>
-      <c r="I184" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="185">
@@ -5752,19 +3544,7 @@
         <v>Characteristics of integrated mangrove-shrimp farming systems in Ben Tre Province, Vietnam: preliminary findings for organic shrimp production certification</v>
       </c>
       <c r="E185" t="str">
-        <v>Ocean and Coastal Research</v>
-      </c>
-      <c r="F185" t="str">
-        <v/>
-      </c>
-      <c r="G185" t="str">
-        <v xml:space="preserve">Thao Huynh Van; Cong Nguyen Van; </v>
-      </c>
-      <c r="H185" t="str">
         <v>2023</v>
-      </c>
-      <c r="I185" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="186">
@@ -5781,19 +3561,7 @@
         <v>Contribution of integrated watershed management (IWM) to disaster risk reduction and community development: Lessons from Nepal</v>
       </c>
       <c r="E186" t="str">
-        <v>International Journal of Disaster Risk Reduction</v>
-      </c>
-      <c r="F186" t="str">
-        <v/>
-      </c>
-      <c r="G186" t="str">
-        <v xml:space="preserve">Thapa Prakash Singh; Chaudhary Sunita; Dasgupta Purnamita; </v>
-      </c>
-      <c r="H186" t="str">
         <v>2022</v>
-      </c>
-      <c r="I186" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="187">
@@ -5810,19 +3578,7 @@
         <v>Understanding the adoption of climate change adaptation strategies among smallholder farmers: Evidence from land reform beneficiaries in South Africa</v>
       </c>
       <c r="E187" t="str">
-        <v>Land Use Policy</v>
-      </c>
-      <c r="F187" t="str">
-        <v/>
-      </c>
-      <c r="G187" t="str">
-        <v xml:space="preserve">Thinda K T; Ogundeji A A; Belle J A; Ojo T O; </v>
-      </c>
-      <c r="H187" t="str">
         <v>2020</v>
-      </c>
-      <c r="I187" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="188">
@@ -5839,19 +3595,7 @@
         <v>Monitoring of ocean surface algal blooms in coastal and oceanic waters around India</v>
       </c>
       <c r="E188" t="str">
-        <v>Environmental Monitoring and Assessment</v>
-      </c>
-      <c r="F188" t="str">
-        <v/>
-      </c>
-      <c r="G188" t="str">
-        <v xml:space="preserve">Tholkapiyan Muniyandi; Shanmugam Palanisamy; Suresh T; </v>
-      </c>
-      <c r="H188" t="str">
         <v>2014</v>
-      </c>
-      <c r="I188" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="189">
@@ -5868,19 +3612,7 @@
         <v>Tolerance diversity in Kabuli chickpea local germplasm ‏under terminal drought</v>
       </c>
       <c r="E189" t="str">
-        <v>Environmental Stresses in Crop Sciences</v>
-      </c>
-      <c r="F189" t="str">
-        <v/>
-      </c>
-      <c r="G189" t="str">
-        <v/>
-      </c>
-      <c r="H189" t="str">
         <v>2022</v>
-      </c>
-      <c r="I189" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="190">
@@ -5897,19 +3629,7 @@
         <v>It takes two to tango: integrating meteorological knowledge and actions for disaster risk reduction</v>
       </c>
       <c r="E190" t="str">
-        <v>Climate and Development</v>
-      </c>
-      <c r="F190" t="str">
-        <v/>
-      </c>
-      <c r="G190" t="str">
-        <v xml:space="preserve">Ton Khanh That; Gaillard J C; Cadag Jake Rom; Naing Aivin; </v>
-      </c>
-      <c r="H190" t="str">
         <v>2017</v>
-      </c>
-      <c r="I190" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="191">
@@ -5926,19 +3646,7 @@
         <v>Assessing livelihood vulnerability of minority ethnic groups to climate change: A case study from the northwest mountainous regions of vietnam</v>
       </c>
       <c r="E191" t="str">
-        <v>Sustainability Switzerland</v>
-      </c>
-      <c r="F191" t="str">
-        <v/>
-      </c>
-      <c r="G191" t="str">
-        <v xml:space="preserve">Tran Van Thanh; An-Vo Duc-Anh; Cockfield Geoff; Mushtaq Shahbaz; </v>
-      </c>
-      <c r="H191" t="str">
         <v>2021</v>
-      </c>
-      <c r="I191" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="192">
@@ -5955,19 +3663,7 @@
         <v>Land use change in the Vietnamese Mekong Delta: New evidence from remote sensing</v>
       </c>
       <c r="E192" t="str">
-        <v>Science of the Total Environment</v>
-      </c>
-      <c r="F192" t="str">
-        <v/>
-      </c>
-      <c r="G192" t="str">
-        <v xml:space="preserve">Vu Hoang Thai Duong; Tran Dung Duc; Schenk Andreas; Nguyen Canh Phuc; Vu Huu Long; Oberle Peter; Trinh Van Cong; Nestmann Franz; </v>
-      </c>
-      <c r="H192" t="str">
         <v>2022</v>
-      </c>
-      <c r="I192" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="193">
@@ -5984,19 +3680,7 @@
         <v>How do smallholder farmers run towards agricultural modernization under multiple stressors in China's coastal zones: an agent-based modeling approach</v>
       </c>
       <c r="E193" t="str">
-        <v>Environment Development and Sustainability</v>
-      </c>
-      <c r="F193" t="str">
-        <v/>
-      </c>
-      <c r="G193" t="str">
-        <v xml:space="preserve">Wang Han; Li Fengqin; Zou Yuhuan; Yang Mengshi; Chen Zhoupeng; Nie Xin; </v>
-      </c>
-      <c r="H193" t="str">
         <v>2024</v>
-      </c>
-      <c r="I193" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="194">
@@ -6013,19 +3697,7 @@
         <v>Impact of current and historical climate shocks on crop diversification in Zambia: Insights from household- and district-level observations</v>
       </c>
       <c r="E194" t="str">
-        <v>Climate Risk Management</v>
-      </c>
-      <c r="F194" t="str">
-        <v/>
-      </c>
-      <c r="G194" t="str">
-        <v xml:space="preserve">Wang Junren; Konar Megan; Anderson Patrese Nicole; Hadunka Protensia; Mulenga Brian; </v>
-      </c>
-      <c r="H194" t="str">
         <v>2025</v>
-      </c>
-      <c r="I194" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="195">
@@ -6042,19 +3714,7 @@
         <v>Cocoa production in West Africa, a review and analysis of recent developments</v>
       </c>
       <c r="E195" t="str">
-        <v>Njas Wageningen Journal of Life Sciences</v>
-      </c>
-      <c r="F195" t="str">
-        <v/>
-      </c>
-      <c r="G195" t="str">
-        <v xml:space="preserve">Wessel Marius; Quist-Wessel P M. Foluke; </v>
-      </c>
-      <c r="H195" t="str">
         <v>2015</v>
-      </c>
-      <c r="I195" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="196">
@@ -6071,19 +3731,7 @@
         <v>Food processing technology: Case study on the development of rice bioindustry</v>
       </c>
       <c r="E196" t="str">
-        <v>Iop Conference Series Earth and Environmental Science</v>
-      </c>
-      <c r="F196" t="str">
-        <v/>
-      </c>
-      <c r="G196" t="str">
-        <v xml:space="preserve">Widowati S; Luna P; </v>
-      </c>
-      <c r="H196" t="str">
         <v>2019</v>
-      </c>
-      <c r="I196" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="197">
@@ -6100,19 +3748,7 @@
         <v>Spatiotemporal Monitoring of Cyanobacterial Blooms and Aquatic Vegetation in Jiangsu Province Using AI Earth Platform and Sentinel-2 MSI Data (2019–2024)</v>
       </c>
       <c r="E197" t="str">
-        <v>Remote Sensing</v>
-      </c>
-      <c r="F197" t="str">
-        <v/>
-      </c>
-      <c r="G197" t="str">
-        <v xml:space="preserve">Xie Xin; Song Ting; Liu Ge; Wang Tiantian; Yang Qi; </v>
-      </c>
-      <c r="H197" t="str">
         <v>2025</v>
-      </c>
-      <c r="I197" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="198">
@@ -6129,19 +3765,7 @@
         <v>Digital soil mapping of soil total nitrogen based on Landsat 8, Sentinel 2, and WorldView-2 images in smallholder farms in Yellow River Basin, China</v>
       </c>
       <c r="E198" t="str">
-        <v>Environmental Monitoring and Assessment</v>
-      </c>
-      <c r="F198" t="str">
-        <v/>
-      </c>
-      <c r="G198" t="str">
-        <v xml:space="preserve">Xu Yiming; Li Bin; Shen Xianbao; Li Ke; Cao Xinyue; Cui Guannan; Yao Zhiliang; </v>
-      </c>
-      <c r="H198" t="str">
         <v>2022</v>
-      </c>
-      <c r="I198" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="199">
@@ -6158,19 +3782,7 @@
         <v>Fish diversity and spatial distribution pattern in the Nujiang River Basin</v>
       </c>
       <c r="E199" t="str">
-        <v>Biodiversity Science</v>
-      </c>
-      <c r="F199" t="str">
-        <v/>
-      </c>
-      <c r="G199" t="str">
-        <v xml:space="preserve">Yang Ke; Ding Chengzhi; Chen Xiaoyong; Ding Liuyong; Huang Minrui; Chen Jinnan; Tao Juan; </v>
-      </c>
-      <c r="H199" t="str">
         <v>2022</v>
-      </c>
-      <c r="I199" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="200">
@@ -6187,19 +3799,7 @@
         <v>The Aplication of Landsat 8 OLI for Total Suspended Solid (TSS) Mapping in Gajahmungkur Reservoir Wonogiri Regency 2016</v>
       </c>
       <c r="E200" t="str">
-        <v>Iop Conference Series Earth and Environmental Science</v>
-      </c>
-      <c r="F200" t="str">
-        <v/>
-      </c>
-      <c r="G200" t="str">
-        <v xml:space="preserve">Yanti Apriwida; Susilo Bowo; Wicaksono Pramaditya; </v>
-      </c>
-      <c r="H200" t="str">
         <v>2016</v>
-      </c>
-      <c r="I200" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="201">
@@ -6216,19 +3816,7 @@
         <v>Year in Review: Beet Growing and Sugar Campaign 2021/2022 in Slovakia</v>
       </c>
       <c r="E201" t="str">
-        <v>Listy Cukrovarnicke A Reparske</v>
-      </c>
-      <c r="F201" t="str">
-        <v/>
-      </c>
-      <c r="G201" t="str">
-        <v/>
-      </c>
-      <c r="H201" t="str">
         <v>2022</v>
-      </c>
-      <c r="I201" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="202">
@@ -6245,19 +3833,7 @@
         <v>The Role of Climate Change Perceptions in Sustainable Agricultural Development: Evidence from Conservation Tillage Technology Adoption in Northern China</v>
       </c>
       <c r="E202" t="str">
-        <v>Land</v>
-      </c>
-      <c r="F202" t="str">
-        <v/>
-      </c>
-      <c r="G202" t="str">
-        <v xml:space="preserve">Yu Leshan; Shi Hengtong; Wu Haixia; Hu Xiangmiao; Ge Yan; Yu Leshui; Cao Wenyu; </v>
-      </c>
-      <c r="H202" t="str">
         <v>2024</v>
-      </c>
-      <c r="I202" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="203">
@@ -6274,19 +3850,7 @@
         <v>On the role of rainfall deficits and cropping choices in loss of agricultural yield in Marathwada, India</v>
       </c>
       <c r="E203" t="str">
-        <v>Environmental Research Letters</v>
-      </c>
-      <c r="F203" t="str">
-        <v/>
-      </c>
-      <c r="G203" t="str">
-        <v xml:space="preserve">Zachariah Mariam; Mondal Arpita; Das Mainak; AchutaRao Krishna Mirle; Ghosh Subimal; </v>
-      </c>
-      <c r="H203" t="str">
         <v>2020</v>
-      </c>
-      <c r="I203" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="204">
@@ -6303,19 +3867,7 @@
         <v>The contribution of cooperative irrigation scheme to poverty reduction in Tanzania</v>
       </c>
       <c r="E204" t="str">
-        <v>Journal of Integrative Agriculture</v>
-      </c>
-      <c r="F204" t="str">
-        <v/>
-      </c>
-      <c r="G204" t="str">
-        <v xml:space="preserve">ZHANG Chuan-hong; BENJAMIN Wandella Amos; WANG Miao; </v>
-      </c>
-      <c r="H204" t="str">
         <v>2021</v>
-      </c>
-      <c r="I204" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="205">
@@ -6332,19 +3884,7 @@
         <v>The impact of climate change on maize production: Empirical findings and implications for sustainable agricultural development</v>
       </c>
       <c r="E205" t="str">
-        <v>Frontiers in Environmental Science</v>
-      </c>
-      <c r="F205" t="str">
-        <v/>
-      </c>
-      <c r="G205" t="str">
-        <v xml:space="preserve">Zhang Zhexi; Wei Jiashuo; Li Jinkai; Jia Yuankai; Wang Wei; Li Jie; Lei Ze; Gao Ming; </v>
-      </c>
-      <c r="H205" t="str">
         <v>2022</v>
-      </c>
-      <c r="I205" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
     <row r="206">
@@ -6361,24 +3901,12 @@
         <v>Why the uncertain term occurs in the farmland lease market: Evidence from rural China</v>
       </c>
       <c r="E206" t="str">
-        <v>Sustainability Switzerland</v>
-      </c>
-      <c r="F206" t="str">
-        <v/>
-      </c>
-      <c r="G206" t="str">
-        <v xml:space="preserve">Zou Baoling; Luo Biliang; </v>
-      </c>
-      <c r="H206" t="str">
         <v>2018</v>
-      </c>
-      <c r="I206" t="str">
-        <v>Journal, Article</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I206"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E206"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>